<commit_message>
make like behavior model for c
</commit_message>
<xml_diff>
--- a/project/nystromformer_timingchart.xlsx
+++ b/project/nystromformer_timingchart.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/furuta/LALSIE/GPT/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6CECA1-AE7C-7C46-94D3-D078D64FB9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3FDEE-66C9-3940-9526-870E475C8C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="4" xr2:uid="{71DF794F-EDEF-1649-A071-280480E3C700}"/>
+    <workbookView xWindow="14780" yWindow="920" windowWidth="14460" windowHeight="18040" activeTab="6" xr2:uid="{71DF794F-EDEF-1649-A071-280480E3C700}"/>
   </bookViews>
   <sheets>
     <sheet name="timing_chart" sheetId="1" r:id="rId1"/>
     <sheet name="data_flow" sheetId="2" r:id="rId2"/>
     <sheet name="landmark" sheetId="4" r:id="rId3"/>
     <sheet name="pipeline_fast" sheetId="5" r:id="rId4"/>
-    <sheet name="data_flow_nonparallel" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="data_flow_nonparallel_ " sheetId="6" r:id="rId6"/>
+    <sheet name="timingchart_small" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="503">
   <si>
     <t>Query</t>
     <phoneticPr fontId="1"/>
@@ -1893,18 +1896,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>get_landm</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>acc + q[0,0]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>acc * 1/75</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>acc &lt;- 0</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1913,42 +1908,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>q[0,74]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>q[0,73]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>q_landmark[0,0]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>acc + q[0,73]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>acc + q[0,74]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>q[0,75]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>divide</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>from memory</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>q[0,76]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>state</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1962,6 +1921,153 @@
   </si>
   <si>
     <t>READ_ACCUM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>memory read</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>memory write</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>acc &gt;&gt; 6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q_landmarls[0,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>read_addr_i</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>read_addr_j</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[63,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[62,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>acc + q[62,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>acc + q[63,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>write_addr_i</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>write_addr_j</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>counter_accum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[127,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[64,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[65,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[126,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>acc + q[64,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>acc + q[126,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>acc + q[127,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q_landmarks[1,0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n = 256</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m = 4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>d = 256</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>clock</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>frequency</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>50MHz ??</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>get_landmark</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>linear</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit width</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>weight</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16bit ??</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[0,0] * w_q[0,0]</t>
+  </si>
+  <si>
+    <t>acc[0] + mul</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w_q[0,1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q[0,0] * w_q[0,1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>acc[1] + mul</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2284,7 +2390,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2453,27 +2559,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -3713,7 +3835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E22F4D36-D49D-5B47-8E31-30E2FA2CE0B7}">
   <dimension ref="A2:AK19"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="82" workbookViewId="0">
+    <sheetView zoomScale="82" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -4611,11 +4733,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7835DD1D-F7B5-F140-896C-73723E09F699}">
   <dimension ref="A1:BG206"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="50" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="N42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="AG94" sqref="AG94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.7109375" defaultRowHeight="20"/>
@@ -7471,17 +7593,17 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C1:AX1 AZ1:XFD1 C2:XFD93 AI51:XFD95 C81:O95 W81:X95 AE81:AE95 C94:AG94 C95:XFD120 C121:AG121 AI121:XFD121 C122:XFD124 C125:AI125 AL125:XFD125 AK125:AK126 C126:XFD137 C138:AL138 AN138:XFD138 C139:XFD142 C143:AO143 AQ143:XFD143 C144:XFD157 C158:AS158 AU158:XFD158 C159:XFD185 C186:AX186 AZ186 BB186:XFD188 C187:BA189 BA189:XFD189 C190:XFD196 C197:BC197 BE197:XFD197 C198:XFD1048576">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>C1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:H37">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>H33&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y55:AD57">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>Y55&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7491,160 +7613,588 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4AFF3BA-0A5F-4E44-9849-23828988BDB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484F7EE6-9ED1-BC4B-8F26-13E64BE2992D}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:AZ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScale="59" workbookViewId="0">
+      <pane xSplit="2" ySplit="8" topLeftCell="AL13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="AQ35" sqref="AQ35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="20"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="40" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="59" customWidth="1"/>
-    <col min="4" max="16384" width="20.7109375" style="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="20.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50">
+      <c r="A2" s="55" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50">
+      <c r="A3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50">
+      <c r="A4" s="55" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50">
+      <c r="A5" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="56">
-        <v>300</v>
-      </c>
-      <c r="C2" s="60"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="40">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="5" customFormat="1">
-      <c r="A5" t="s">
+    <row r="6" spans="1:50">
+      <c r="A6" s="55" t="s">
+        <v>487</v>
+      </c>
+      <c r="B6" s="55"/>
+    </row>
+    <row r="7" spans="1:50">
+      <c r="A7" s="55" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50">
+      <c r="A8" s="55" t="s">
+        <v>489</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>490</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN8" s="1">
+        <v>64</v>
+      </c>
+      <c r="AO8" s="1">
+        <v>65</v>
+      </c>
+      <c r="AP8" s="1">
+        <v>66</v>
+      </c>
+      <c r="AQ8" s="1">
+        <v>67</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>68</v>
+      </c>
+      <c r="AS8" s="1">
+        <v>69</v>
+      </c>
+      <c r="AT8" s="1">
+        <v>70</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV8" s="1">
+        <v>132</v>
+      </c>
+      <c r="AW8" s="1">
+        <v>133</v>
+      </c>
+      <c r="AX8" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50">
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
+    </row>
+    <row r="10" spans="1:50">
+      <c r="A10" s="55"/>
+      <c r="B10" s="55"/>
+    </row>
+    <row r="11" spans="1:50">
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+    </row>
+    <row r="12" spans="1:50">
+      <c r="A12" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B12" t="s">
+        <v>470</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50">
+      <c r="B13" t="s">
+        <v>471</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50">
+      <c r="B14" t="s">
+        <v>466</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:50">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="56"/>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:51">
+      <c r="B17" t="s">
+        <v>496</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51">
+      <c r="B18" t="s">
+        <v>185</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51">
+      <c r="B19" t="s">
+        <v>461</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51">
+      <c r="B22" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="23" spans="1:51">
+      <c r="B23" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="24" spans="1:51">
+      <c r="B24" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="27" spans="1:51">
+      <c r="A27" t="s">
+        <v>493</v>
+      </c>
+      <c r="B27" t="s">
+        <v>462</v>
+      </c>
+      <c r="AJ27" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="AK27" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="AQ27" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="AR27" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="AX27" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="AY27" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="28" spans="1:51">
+      <c r="B28" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51">
+      <c r="B31" t="s">
+        <v>470</v>
+      </c>
+      <c r="AK31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN31" s="1">
+        <v>63</v>
+      </c>
+      <c r="AR31" s="1">
+        <v>64</v>
+      </c>
+      <c r="AS31" s="1">
+        <v>65</v>
+      </c>
+      <c r="AT31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU31" s="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51">
+      <c r="B32" t="s">
+        <v>471</v>
+      </c>
+      <c r="AK32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:52">
+      <c r="A33" s="1"/>
+      <c r="B33" t="s">
+        <v>466</v>
+      </c>
+      <c r="AK33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN33" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="AR33" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AS33" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="AT33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU33" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="34" spans="1:52">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:52">
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO35" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="AP35" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="AT35" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AU35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV35" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="AW35" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="36" spans="1:52">
+      <c r="B36" t="s">
+        <v>461</v>
+      </c>
+      <c r="AK36" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="AM36" s="50" t="s">
         <v>459</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>473</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="AN36" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO36" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="AP36" s="50" t="s">
+        <v>475</v>
+      </c>
+      <c r="AR36" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="AT36" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="AU36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV36" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AW36" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AY36" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="37" spans="1:52">
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ37" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="AX37" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="39" spans="1:52">
+      <c r="B39" t="s">
         <v>476</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="58" customFormat="1">
-      <c r="A6"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="59"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1"/>
-      <c r="B7" s="40" t="s">
-        <v>471</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="K7" s="44" t="s">
+      <c r="AS39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:52">
+      <c r="B40" t="s">
+        <v>477</v>
+      </c>
+      <c r="AS40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:52">
+      <c r="B41" t="s">
+        <v>467</v>
+      </c>
+      <c r="AS41" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="B9" s="40" t="s">
-        <v>463</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>460</v>
-      </c>
-      <c r="F9" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="50" t="s">
-        <v>467</v>
-      </c>
-      <c r="H9" s="50" t="s">
-        <v>468</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10" s="40" t="s">
-        <v>470</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="B11" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>466</v>
+      <c r="AZ41" s="1" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F16:G16"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="D7:H7 E8:I8 D1:XFD4 D6:XFD6 D5:G5 I5:XFD5 D11:H12 J11:XFD12 L7:XFD7 D10:XFD10 D9:K9 M9:XFD9 K8:XFD8 D20:XFD1048576 D19:H19 J19:XFD19 D13:XFD18">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>D1&lt;&gt;""</formula>
+  <conditionalFormatting sqref="C9:XFD15 C16:F16 I16:XFD16 C17:XFD1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>C9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120B20A9-82A7-4D47-8C93-28558266A36A}">
+  <dimension ref="A1:AP36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="20.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="55" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="55" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="55" t="s">
+        <v>487</v>
+      </c>
+      <c r="B6" s="55"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="55" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="55" t="s">
+        <v>489</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="55"/>
+      <c r="B10" s="55"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="2"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16"/>
+    </row>
+    <row r="33" spans="1:42">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:42">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="36" spans="1:42">
+      <c r="AM36" s="50"/>
+      <c r="AN36" s="50"/>
+      <c r="AO36" s="50"/>
+      <c r="AP36" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F16:G16"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="C9:XFD15 C16:F16 I16:XFD16 C17:XFD1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C9&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB43E1E-775C-124D-AAB8-6548FC785F0F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update timing chart (only address change)
</commit_message>
<xml_diff>
--- a/project/nystromformer_timingchart.xlsx
+++ b/project/nystromformer_timingchart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/furuta/LALSIE/GPT/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF11565-1CBE-BE45-B8FB-55739AD86152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2065AF81-7E05-6444-A6E1-D8AD58973475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" firstSheet="3" activeTab="6" xr2:uid="{71DF794F-EDEF-1649-A071-280480E3C700}"/>
+    <workbookView xWindow="14760" yWindow="920" windowWidth="14480" windowHeight="18060" firstSheet="3" activeTab="6" xr2:uid="{71DF794F-EDEF-1649-A071-280480E3C700}"/>
   </bookViews>
   <sheets>
     <sheet name="timing_chart" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="525">
   <si>
     <t>Query</t>
     <phoneticPr fontId="1"/>
@@ -2128,6 +2128,32 @@
   </si>
   <si>
     <t>255 (n-1)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>iterative_inv_V0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3 (m-1)</t>
+  </si>
+  <si>
+    <t>l</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>matmul_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1 * 2^T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>255 (n-1)</t>
+  </si>
+  <si>
+    <t>k3 * v</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2492,7 +2518,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2664,13 +2690,22 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2691,7 +2726,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2700,23 +2738,14 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7947,10 +7976,10 @@
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="57" t="s">
+      <c r="F16" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="57"/>
+      <c r="G16" s="61"/>
       <c r="H16"/>
     </row>
     <row r="17" spans="1:51">
@@ -8238,13 +8267,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120B20A9-82A7-4D47-8C93-28558266A36A}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:DR35"/>
+  <dimension ref="A1:IR35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="DG6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="R23" sqref="R23"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20"/>
@@ -8254,23 +8283,23 @@
     <col min="3" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:122">
+    <row r="1" spans="1:252">
       <c r="A1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:122">
+    <row r="2" spans="1:252">
       <c r="A2" s="55" t="s">
         <v>487</v>
       </c>
       <c r="B2" s="55"/>
     </row>
-    <row r="3" spans="1:122">
+    <row r="3" spans="1:252">
       <c r="A3" s="55" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="4" spans="1:122" ht="21" customHeight="1">
+    <row r="4" spans="1:252" ht="21" customHeight="1">
       <c r="A4" s="55" t="s">
         <v>489</v>
       </c>
@@ -8278,615 +8307,983 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:122" s="74" customFormat="1" ht="21" customHeight="1">
-      <c r="A5" s="70"/>
-      <c r="B5" s="70" t="s">
+    <row r="5" spans="1:252" s="60" customFormat="1" ht="21" customHeight="1">
+      <c r="A5" s="59"/>
+      <c r="B5" s="59" t="s">
         <v>462</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="74" t="s">
         <v>507</v>
       </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71" t="s">
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74" t="s">
         <v>508</v>
       </c>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
-      <c r="U5" s="71"/>
-      <c r="V5" s="71"/>
-      <c r="W5" s="71"/>
-      <c r="X5" s="71"/>
-      <c r="Y5" s="71"/>
-      <c r="Z5" s="71"/>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="71"/>
-      <c r="AC5" s="71"/>
-      <c r="AD5" s="71"/>
-      <c r="AE5" s="71"/>
-      <c r="AF5" s="71"/>
-      <c r="AG5" s="71" t="s">
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="74"/>
+      <c r="AE5" s="74"/>
+      <c r="AF5" s="74"/>
+      <c r="AG5" s="74" t="s">
         <v>509</v>
       </c>
-      <c r="AH5" s="71"/>
-      <c r="AI5" s="71"/>
-      <c r="AJ5" s="71"/>
-      <c r="AK5" s="71"/>
-      <c r="AL5" s="71"/>
-      <c r="AM5" s="71"/>
-      <c r="AN5" s="71"/>
-      <c r="AO5" s="71"/>
-      <c r="AP5" s="71"/>
-      <c r="AQ5" s="71"/>
-      <c r="AR5" s="71"/>
-      <c r="AS5" s="71"/>
-      <c r="AT5" s="71"/>
-      <c r="AU5" s="71"/>
-      <c r="AV5" s="72" t="s">
+      <c r="AH5" s="74"/>
+      <c r="AI5" s="74"/>
+      <c r="AJ5" s="74"/>
+      <c r="AK5" s="74"/>
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="74"/>
+      <c r="AN5" s="74"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74"/>
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="74"/>
+      <c r="AT5" s="74"/>
+      <c r="AU5" s="74"/>
+      <c r="AV5" s="73" t="s">
         <v>510</v>
       </c>
-      <c r="AW5" s="72"/>
-      <c r="AX5" s="72"/>
-      <c r="AY5" s="72"/>
-      <c r="AZ5" s="72"/>
-      <c r="BA5" s="72"/>
-      <c r="BB5" s="72"/>
-      <c r="BC5" s="72"/>
-      <c r="BD5" s="72"/>
-      <c r="BE5" s="72"/>
-      <c r="BF5" s="72"/>
-      <c r="BG5" s="72"/>
-      <c r="BH5" s="72"/>
-      <c r="BI5" s="72"/>
-      <c r="BJ5" s="72"/>
-      <c r="BK5" s="72" t="s">
+      <c r="AW5" s="73"/>
+      <c r="AX5" s="73"/>
+      <c r="AY5" s="73"/>
+      <c r="AZ5" s="73"/>
+      <c r="BA5" s="73"/>
+      <c r="BB5" s="73"/>
+      <c r="BC5" s="73"/>
+      <c r="BD5" s="73"/>
+      <c r="BE5" s="73"/>
+      <c r="BF5" s="73"/>
+      <c r="BG5" s="73"/>
+      <c r="BH5" s="73"/>
+      <c r="BI5" s="73"/>
+      <c r="BJ5" s="73"/>
+      <c r="BK5" s="73" t="s">
         <v>511</v>
       </c>
-      <c r="BL5" s="72"/>
-      <c r="BM5" s="72"/>
-      <c r="BN5" s="72"/>
-      <c r="BO5" s="72"/>
-      <c r="BP5" s="72"/>
-      <c r="BQ5" s="72"/>
-      <c r="BR5" s="72"/>
-      <c r="BS5" s="72"/>
-      <c r="BT5" s="72"/>
-      <c r="BU5" s="72"/>
-      <c r="BV5" s="72"/>
-      <c r="BW5" s="72"/>
-      <c r="BX5" s="72"/>
-      <c r="BY5" s="72"/>
-      <c r="BZ5" s="73" t="s">
+      <c r="BL5" s="73"/>
+      <c r="BM5" s="73"/>
+      <c r="BN5" s="73"/>
+      <c r="BO5" s="73"/>
+      <c r="BP5" s="73"/>
+      <c r="BQ5" s="73"/>
+      <c r="BR5" s="73"/>
+      <c r="BS5" s="73"/>
+      <c r="BT5" s="73"/>
+      <c r="BU5" s="73"/>
+      <c r="BV5" s="73"/>
+      <c r="BW5" s="73"/>
+      <c r="BX5" s="73"/>
+      <c r="BY5" s="73"/>
+      <c r="BZ5" s="62" t="s">
         <v>513</v>
       </c>
-      <c r="CA5" s="73"/>
-      <c r="CB5" s="73"/>
-      <c r="CC5" s="73"/>
-      <c r="CD5" s="73"/>
-      <c r="CE5" s="73"/>
-      <c r="CF5" s="73"/>
-      <c r="CG5" s="73"/>
-      <c r="CH5" s="73"/>
-      <c r="CI5" s="73"/>
-      <c r="CJ5" s="73"/>
-      <c r="CK5" s="73"/>
-      <c r="CL5" s="73"/>
-      <c r="CM5" s="73"/>
-      <c r="CN5" s="73"/>
-      <c r="CO5" s="73" t="s">
+      <c r="CA5" s="62"/>
+      <c r="CB5" s="62"/>
+      <c r="CC5" s="62"/>
+      <c r="CD5" s="62"/>
+      <c r="CE5" s="62"/>
+      <c r="CF5" s="62"/>
+      <c r="CG5" s="62"/>
+      <c r="CH5" s="62"/>
+      <c r="CI5" s="62"/>
+      <c r="CJ5" s="62"/>
+      <c r="CK5" s="62"/>
+      <c r="CL5" s="62"/>
+      <c r="CM5" s="62"/>
+      <c r="CN5" s="62"/>
+      <c r="CO5" s="62" t="s">
         <v>515</v>
       </c>
-      <c r="CP5" s="73"/>
-      <c r="CQ5" s="73"/>
-      <c r="CR5" s="73"/>
-      <c r="CS5" s="73"/>
-      <c r="CT5" s="73"/>
-      <c r="CU5" s="73"/>
-      <c r="CV5" s="73"/>
-      <c r="CW5" s="73"/>
-      <c r="CX5" s="73"/>
-      <c r="CY5" s="73"/>
-      <c r="CZ5" s="73"/>
-      <c r="DA5" s="73"/>
-      <c r="DB5" s="73"/>
-      <c r="DC5" s="73"/>
-      <c r="DD5" s="73" t="s">
+      <c r="CP5" s="62"/>
+      <c r="CQ5" s="62"/>
+      <c r="CR5" s="62"/>
+      <c r="CS5" s="62"/>
+      <c r="CT5" s="62"/>
+      <c r="CU5" s="62"/>
+      <c r="CV5" s="62"/>
+      <c r="CW5" s="62"/>
+      <c r="CX5" s="62"/>
+      <c r="CY5" s="62"/>
+      <c r="CZ5" s="62"/>
+      <c r="DA5" s="62"/>
+      <c r="DB5" s="62"/>
+      <c r="DC5" s="62"/>
+      <c r="DD5" s="62" t="s">
         <v>516</v>
       </c>
-      <c r="DE5" s="73"/>
-      <c r="DF5" s="73"/>
-      <c r="DG5" s="73"/>
-      <c r="DH5" s="73"/>
-      <c r="DI5" s="73"/>
-      <c r="DJ5" s="73"/>
-      <c r="DK5" s="73"/>
-      <c r="DL5" s="73"/>
-      <c r="DM5" s="73"/>
-      <c r="DN5" s="73"/>
-      <c r="DO5" s="73"/>
-      <c r="DP5" s="73"/>
-      <c r="DQ5" s="73"/>
-      <c r="DR5" s="73"/>
-    </row>
-    <row r="7" spans="1:122" ht="21" customHeight="1">
+      <c r="DE5" s="62"/>
+      <c r="DF5" s="62"/>
+      <c r="DG5" s="62"/>
+      <c r="DH5" s="62"/>
+      <c r="DI5" s="62"/>
+      <c r="DJ5" s="62"/>
+      <c r="DK5" s="62"/>
+      <c r="DL5" s="62"/>
+      <c r="DM5" s="62"/>
+      <c r="DN5" s="62"/>
+      <c r="DO5" s="62"/>
+      <c r="DP5" s="62"/>
+      <c r="DQ5" s="62"/>
+      <c r="DR5" s="62"/>
+      <c r="DS5" s="60" t="s">
+        <v>518</v>
+      </c>
+      <c r="EN5" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="FC5" s="60" t="s">
+        <v>404</v>
+      </c>
+      <c r="FR5" s="60" t="s">
+        <v>410</v>
+      </c>
+      <c r="GG5" s="60" t="s">
+        <v>521</v>
+      </c>
+      <c r="GZ5" s="60" t="s">
+        <v>522</v>
+      </c>
+      <c r="HO5" s="60" t="s">
+        <v>524</v>
+      </c>
+      <c r="ID5" s="60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:252" ht="21" customHeight="1">
       <c r="A7" s="55"/>
       <c r="B7" s="55"/>
     </row>
-    <row r="8" spans="1:122">
+    <row r="8" spans="1:252">
       <c r="A8" s="55" t="s">
         <v>503</v>
       </c>
       <c r="B8" s="55" t="s">
         <v>504</v>
       </c>
-      <c r="C8" s="60">
-        <v>0</v>
-      </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
+      <c r="C8" s="63">
+        <v>0</v>
+      </c>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="65"/>
       <c r="J8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="63" t="s">
+      <c r="K8" s="66" t="s">
         <v>517</v>
       </c>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="60">
-        <v>0</v>
-      </c>
-      <c r="S8" s="61"/>
-      <c r="T8" s="61"/>
-      <c r="U8" s="61"/>
-      <c r="V8" s="61"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="62"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="63">
+        <v>0</v>
+      </c>
+      <c r="S8" s="64"/>
+      <c r="T8" s="64"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="64"/>
+      <c r="X8" s="65"/>
       <c r="Y8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="63" t="s">
+      <c r="Z8" s="66" t="s">
         <v>517</v>
       </c>
-      <c r="AA8" s="64"/>
-      <c r="AB8" s="64"/>
-      <c r="AC8" s="64"/>
-      <c r="AD8" s="64"/>
-      <c r="AE8" s="64"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="60">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="61"/>
-      <c r="AI8" s="61"/>
-      <c r="AJ8" s="61"/>
-      <c r="AK8" s="61"/>
-      <c r="AL8" s="61"/>
-      <c r="AM8" s="62"/>
+      <c r="AA8" s="67"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="68"/>
+      <c r="AG8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="64"/>
+      <c r="AI8" s="64"/>
+      <c r="AJ8" s="64"/>
+      <c r="AK8" s="64"/>
+      <c r="AL8" s="64"/>
+      <c r="AM8" s="65"/>
       <c r="AN8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AO8" s="63" t="s">
+      <c r="AO8" s="66" t="s">
         <v>517</v>
       </c>
-      <c r="AP8" s="64"/>
-      <c r="AQ8" s="64"/>
-      <c r="AR8" s="64"/>
-      <c r="AS8" s="64"/>
-      <c r="AT8" s="64"/>
-      <c r="AU8" s="65"/>
-      <c r="AV8" s="66">
+      <c r="AP8" s="67"/>
+      <c r="AQ8" s="67"/>
+      <c r="AR8" s="67"/>
+      <c r="AS8" s="67"/>
+      <c r="AT8" s="67"/>
+      <c r="AU8" s="68"/>
+      <c r="AV8" s="57">
         <v>0</v>
       </c>
       <c r="AW8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AX8" s="67">
+      <c r="AX8" s="58">
         <v>63</v>
       </c>
       <c r="AY8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="AZ8" s="66">
+      <c r="AZ8" s="57">
         <v>0</v>
       </c>
       <c r="BA8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BB8" s="67">
+      <c r="BB8" s="58">
         <v>63</v>
       </c>
       <c r="BC8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BD8" s="66">
+      <c r="BD8" s="57">
         <v>192</v>
       </c>
       <c r="BE8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BF8" s="67">
+      <c r="BF8" s="58">
         <v>255</v>
       </c>
       <c r="BG8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BH8" s="66">
+      <c r="BH8" s="57">
         <v>192</v>
       </c>
       <c r="BI8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BJ8" s="67">
+      <c r="BJ8" s="58">
         <v>255</v>
       </c>
-      <c r="BK8" s="66">
+      <c r="BK8" s="57">
         <v>0</v>
       </c>
       <c r="BL8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BM8" s="67">
+      <c r="BM8" s="58">
         <v>63</v>
       </c>
       <c r="BN8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BO8" s="66">
+      <c r="BO8" s="57">
         <v>0</v>
       </c>
       <c r="BP8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BQ8" s="67">
+      <c r="BQ8" s="58">
         <v>63</v>
       </c>
       <c r="BR8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BS8" s="66">
+      <c r="BS8" s="57">
         <v>192</v>
       </c>
       <c r="BT8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BU8" s="67">
+      <c r="BU8" s="58">
         <v>255</v>
       </c>
       <c r="BV8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BW8" s="66">
+      <c r="BW8" s="57">
         <v>192</v>
       </c>
       <c r="BX8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BY8" s="67">
+      <c r="BY8" s="58">
         <v>255</v>
       </c>
-      <c r="BZ8" s="60">
-        <v>0</v>
-      </c>
-      <c r="CA8" s="61"/>
-      <c r="CB8" s="61"/>
-      <c r="CC8" s="61"/>
-      <c r="CD8" s="61"/>
-      <c r="CE8" s="61"/>
-      <c r="CF8" s="62"/>
+      <c r="BZ8" s="63">
+        <v>0</v>
+      </c>
+      <c r="CA8" s="64"/>
+      <c r="CB8" s="64"/>
+      <c r="CC8" s="64"/>
+      <c r="CD8" s="64"/>
+      <c r="CE8" s="64"/>
+      <c r="CF8" s="65"/>
       <c r="CG8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="CH8" s="63" t="s">
+      <c r="CH8" s="66" t="s">
         <v>517</v>
       </c>
-      <c r="CI8" s="64"/>
-      <c r="CJ8" s="64"/>
-      <c r="CK8" s="64"/>
-      <c r="CL8" s="64"/>
-      <c r="CM8" s="64"/>
-      <c r="CN8" s="65"/>
-      <c r="CO8" s="60">
-        <v>0</v>
-      </c>
-      <c r="CP8" s="61"/>
-      <c r="CQ8" s="61"/>
-      <c r="CR8" s="61"/>
-      <c r="CS8" s="61"/>
-      <c r="CT8" s="61"/>
-      <c r="CU8" s="62"/>
+      <c r="CI8" s="67"/>
+      <c r="CJ8" s="67"/>
+      <c r="CK8" s="67"/>
+      <c r="CL8" s="67"/>
+      <c r="CM8" s="67"/>
+      <c r="CN8" s="68"/>
+      <c r="CO8" s="63">
+        <v>0</v>
+      </c>
+      <c r="CP8" s="64"/>
+      <c r="CQ8" s="64"/>
+      <c r="CR8" s="64"/>
+      <c r="CS8" s="64"/>
+      <c r="CT8" s="64"/>
+      <c r="CU8" s="65"/>
       <c r="CV8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="CW8" s="63" t="s">
+      <c r="CW8" s="66" t="s">
         <v>514</v>
       </c>
-      <c r="CX8" s="64"/>
-      <c r="CY8" s="64"/>
-      <c r="CZ8" s="64"/>
-      <c r="DA8" s="64"/>
-      <c r="DB8" s="64"/>
-      <c r="DC8" s="65"/>
-      <c r="DD8" s="60">
-        <v>0</v>
-      </c>
-      <c r="DE8" s="61"/>
-      <c r="DF8" s="61"/>
-      <c r="DG8" s="61"/>
-      <c r="DH8" s="61"/>
-      <c r="DI8" s="61"/>
-      <c r="DJ8" s="62"/>
+      <c r="CX8" s="67"/>
+      <c r="CY8" s="67"/>
+      <c r="CZ8" s="67"/>
+      <c r="DA8" s="67"/>
+      <c r="DB8" s="67"/>
+      <c r="DC8" s="68"/>
+      <c r="DD8" s="63">
+        <v>0</v>
+      </c>
+      <c r="DE8" s="64"/>
+      <c r="DF8" s="64"/>
+      <c r="DG8" s="64"/>
+      <c r="DH8" s="64"/>
+      <c r="DI8" s="64"/>
+      <c r="DJ8" s="65"/>
       <c r="DK8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="DL8" s="63" t="s">
+      <c r="DL8" s="66" t="s">
         <v>514</v>
       </c>
-      <c r="DM8" s="64"/>
-      <c r="DN8" s="64"/>
-      <c r="DO8" s="64"/>
-      <c r="DP8" s="64"/>
-      <c r="DQ8" s="64"/>
-      <c r="DR8" s="65"/>
-    </row>
-    <row r="9" spans="1:122">
+      <c r="DM8" s="67"/>
+      <c r="DN8" s="67"/>
+      <c r="DO8" s="67"/>
+      <c r="DP8" s="67"/>
+      <c r="DQ8" s="67"/>
+      <c r="DR8" s="68"/>
+      <c r="DS8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="DW8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="DZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="ED8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EK8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EV8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FK8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="FY8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FZ8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="GN8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GO8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GV8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="GX8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="HG8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HH8" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="HO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="HV8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HW8" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="ID8" s="45">
+        <v>0</v>
+      </c>
+      <c r="IE8" s="46"/>
+      <c r="IF8" s="46"/>
+      <c r="IG8" s="46"/>
+      <c r="IH8" s="46"/>
+      <c r="II8" s="46"/>
+      <c r="IJ8" s="46"/>
+      <c r="IK8" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IL8" s="45" t="s">
+        <v>523</v>
+      </c>
+      <c r="IM8" s="46"/>
+      <c r="IN8" s="46"/>
+      <c r="IO8" s="46"/>
+      <c r="IP8" s="46"/>
+      <c r="IQ8" s="46"/>
+      <c r="IR8" s="46"/>
+    </row>
+    <row r="9" spans="1:252">
       <c r="A9" s="55"/>
       <c r="B9" s="55" t="s">
         <v>505</v>
       </c>
-      <c r="C9" s="58">
-        <v>0</v>
-      </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
+      <c r="C9" s="69">
+        <v>0</v>
+      </c>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="70" t="s">
         <v>512</v>
       </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
       <c r="J9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="58">
-        <v>0</v>
-      </c>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
+      <c r="K9" s="69">
+        <v>0</v>
+      </c>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
       <c r="N9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="63" t="s">
+      <c r="O9" s="66" t="s">
         <v>512</v>
       </c>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="58">
-        <v>0</v>
-      </c>
-      <c r="S9" s="58"/>
-      <c r="T9" s="58"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="69">
+        <v>0</v>
+      </c>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
       <c r="U9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V9" s="59" t="s">
+      <c r="V9" s="70" t="s">
         <v>512</v>
       </c>
-      <c r="W9" s="59"/>
-      <c r="X9" s="59"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
       <c r="Y9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z9" s="58">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="58"/>
-      <c r="AB9" s="58"/>
+      <c r="Z9" s="69">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
       <c r="AC9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AD9" s="63" t="s">
+      <c r="AD9" s="66" t="s">
         <v>512</v>
       </c>
-      <c r="AE9" s="64"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="58">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="58"/>
-      <c r="AI9" s="58"/>
+      <c r="AE9" s="67"/>
+      <c r="AF9" s="68"/>
+      <c r="AG9" s="69">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="69"/>
+      <c r="AI9" s="69"/>
       <c r="AJ9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AK9" s="59" t="s">
+      <c r="AK9" s="70" t="s">
         <v>512</v>
       </c>
-      <c r="AL9" s="59"/>
-      <c r="AM9" s="59"/>
+      <c r="AL9" s="70"/>
+      <c r="AM9" s="70"/>
       <c r="AN9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AO9" s="58">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="58"/>
-      <c r="AQ9" s="58"/>
+      <c r="AO9" s="69">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="69"/>
+      <c r="AQ9" s="69"/>
       <c r="AR9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AS9" s="63" t="s">
+      <c r="AS9" s="66" t="s">
         <v>512</v>
       </c>
-      <c r="AT9" s="64"/>
-      <c r="AU9" s="65"/>
-      <c r="AV9" s="68">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="68"/>
-      <c r="AX9" s="68"/>
+      <c r="AT9" s="67"/>
+      <c r="AU9" s="68"/>
+      <c r="AV9" s="72">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="72"/>
+      <c r="AX9" s="72"/>
       <c r="AY9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AZ9" s="69">
+      <c r="AZ9" s="71">
         <v>255</v>
       </c>
-      <c r="BA9" s="69"/>
-      <c r="BB9" s="69"/>
+      <c r="BA9" s="71"/>
+      <c r="BB9" s="71"/>
       <c r="BC9" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BD9" s="68">
-        <v>0</v>
-      </c>
-      <c r="BE9" s="68"/>
-      <c r="BF9" s="68"/>
+      <c r="BD9" s="72">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="72"/>
+      <c r="BF9" s="72"/>
       <c r="BG9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BH9" s="69">
+      <c r="BH9" s="71">
         <v>255</v>
       </c>
-      <c r="BI9" s="69"/>
-      <c r="BJ9" s="69"/>
-      <c r="BK9" s="68">
-        <v>0</v>
-      </c>
-      <c r="BL9" s="68"/>
-      <c r="BM9" s="68"/>
+      <c r="BI9" s="71"/>
+      <c r="BJ9" s="71"/>
+      <c r="BK9" s="72">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="72"/>
+      <c r="BM9" s="72"/>
       <c r="BN9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BO9" s="69">
+      <c r="BO9" s="71">
         <v>255</v>
       </c>
-      <c r="BP9" s="69"/>
-      <c r="BQ9" s="69"/>
+      <c r="BP9" s="71"/>
+      <c r="BQ9" s="71"/>
       <c r="BR9" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BS9" s="68">
-        <v>0</v>
-      </c>
-      <c r="BT9" s="68"/>
-      <c r="BU9" s="68"/>
+      <c r="BS9" s="72">
+        <v>0</v>
+      </c>
+      <c r="BT9" s="72"/>
+      <c r="BU9" s="72"/>
       <c r="BV9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BW9" s="69">
+      <c r="BW9" s="71">
         <v>255</v>
       </c>
-      <c r="BX9" s="69"/>
-      <c r="BY9" s="69"/>
-      <c r="BZ9" s="58">
-        <v>0</v>
-      </c>
-      <c r="CA9" s="58"/>
-      <c r="CB9" s="58"/>
+      <c r="BX9" s="71"/>
+      <c r="BY9" s="71"/>
+      <c r="BZ9" s="69">
+        <v>0</v>
+      </c>
+      <c r="CA9" s="69"/>
+      <c r="CB9" s="69"/>
       <c r="CC9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="CD9" s="59" t="s">
+      <c r="CD9" s="70" t="s">
         <v>514</v>
       </c>
-      <c r="CE9" s="59"/>
-      <c r="CF9" s="59"/>
+      <c r="CE9" s="70"/>
+      <c r="CF9" s="70"/>
       <c r="CG9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="CH9" s="58">
-        <v>0</v>
-      </c>
-      <c r="CI9" s="58"/>
-      <c r="CJ9" s="58"/>
+      <c r="CH9" s="69">
+        <v>0</v>
+      </c>
+      <c r="CI9" s="69"/>
+      <c r="CJ9" s="69"/>
       <c r="CK9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="CL9" s="63" t="s">
+      <c r="CL9" s="66" t="s">
         <v>514</v>
       </c>
-      <c r="CM9" s="64"/>
-      <c r="CN9" s="65"/>
-      <c r="CO9" s="58">
-        <v>0</v>
-      </c>
-      <c r="CP9" s="58"/>
-      <c r="CQ9" s="58"/>
+      <c r="CM9" s="67"/>
+      <c r="CN9" s="68"/>
+      <c r="CO9" s="69">
+        <v>0</v>
+      </c>
+      <c r="CP9" s="69"/>
+      <c r="CQ9" s="69"/>
       <c r="CR9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="CS9" s="59" t="s">
+      <c r="CS9" s="70" t="s">
         <v>514</v>
       </c>
-      <c r="CT9" s="59"/>
-      <c r="CU9" s="59"/>
+      <c r="CT9" s="70"/>
+      <c r="CU9" s="70"/>
       <c r="CV9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="CW9" s="58">
-        <v>0</v>
-      </c>
-      <c r="CX9" s="58"/>
-      <c r="CY9" s="58"/>
+      <c r="CW9" s="69">
+        <v>0</v>
+      </c>
+      <c r="CX9" s="69"/>
+      <c r="CY9" s="69"/>
       <c r="CZ9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="DA9" s="63" t="s">
+      <c r="DA9" s="66" t="s">
         <v>514</v>
       </c>
-      <c r="DB9" s="64"/>
-      <c r="DC9" s="65"/>
-      <c r="DD9" s="58">
-        <v>0</v>
-      </c>
-      <c r="DE9" s="58"/>
-      <c r="DF9" s="58"/>
+      <c r="DB9" s="67"/>
+      <c r="DC9" s="68"/>
+      <c r="DD9" s="69">
+        <v>0</v>
+      </c>
+      <c r="DE9" s="69"/>
+      <c r="DF9" s="69"/>
       <c r="DG9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="DH9" s="59" t="s">
+      <c r="DH9" s="70" t="s">
         <v>517</v>
       </c>
-      <c r="DI9" s="59"/>
-      <c r="DJ9" s="59"/>
+      <c r="DI9" s="70"/>
+      <c r="DJ9" s="70"/>
       <c r="DK9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="DL9" s="58">
-        <v>0</v>
-      </c>
-      <c r="DM9" s="58"/>
-      <c r="DN9" s="58"/>
+      <c r="DL9" s="69">
+        <v>0</v>
+      </c>
+      <c r="DM9" s="69"/>
+      <c r="DN9" s="69"/>
       <c r="DO9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="DP9" s="59" t="s">
+      <c r="DP9" s="70" t="s">
         <v>517</v>
       </c>
-      <c r="DQ9" s="59"/>
-      <c r="DR9" s="59"/>
-    </row>
-    <row r="10" spans="1:122">
+      <c r="DQ9" s="70"/>
+      <c r="DR9" s="70"/>
+      <c r="DS9" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="DU9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="DV9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="DW9" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="DY9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="DZ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EB9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EC9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="ED9" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EF9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EG9" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EI9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EJ9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EK9" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EM9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EN9" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="ER9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EU9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EV9" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EZ9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FG9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FJ9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FK9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FN9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FR9" s="1">
+        <v>0</v>
+      </c>
+      <c r="FU9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FV9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FY9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FZ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="GC9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GD9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GG9" s="1">
+        <v>0</v>
+      </c>
+      <c r="GJ9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GN9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="GR9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GV9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW9" s="1">
+        <v>0</v>
+      </c>
+      <c r="GX9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GZ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="HC9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HD9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="HG9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HH9" s="1">
+        <v>0</v>
+      </c>
+      <c r="HK9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HL9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="HO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="HR9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HS9" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="HV9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HW9" s="1">
+        <v>0</v>
+      </c>
+      <c r="HZ9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="IA9" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="ID9" s="45">
+        <v>0</v>
+      </c>
+      <c r="IE9" s="46"/>
+      <c r="IF9" s="46"/>
+      <c r="IG9" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IH9" s="45" t="s">
+        <v>512</v>
+      </c>
+      <c r="II9" s="46"/>
+      <c r="IJ9" s="46"/>
+      <c r="IK9" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IL9" s="45">
+        <v>0</v>
+      </c>
+      <c r="IM9" s="46"/>
+      <c r="IN9" s="46"/>
+      <c r="IO9" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IP9" s="45" t="s">
+        <v>512</v>
+      </c>
+      <c r="IQ9" s="46"/>
+      <c r="IR9" s="46"/>
+    </row>
+    <row r="10" spans="1:252">
       <c r="A10" s="55"/>
       <c r="B10" s="55" t="s">
         <v>506</v>
@@ -9026,48 +9423,48 @@
       <c r="AU10" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="AV10" s="68">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="68"/>
-      <c r="AX10" s="68"/>
-      <c r="AY10" s="68"/>
-      <c r="AZ10" s="68"/>
-      <c r="BA10" s="68"/>
-      <c r="BB10" s="68"/>
+      <c r="AV10" s="72">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="72"/>
+      <c r="AX10" s="72"/>
+      <c r="AY10" s="72"/>
+      <c r="AZ10" s="72"/>
+      <c r="BA10" s="72"/>
+      <c r="BB10" s="72"/>
       <c r="BC10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BD10" s="69">
+      <c r="BD10" s="71">
         <v>4</v>
       </c>
-      <c r="BE10" s="69"/>
-      <c r="BF10" s="69"/>
-      <c r="BG10" s="69"/>
-      <c r="BH10" s="69"/>
-      <c r="BI10" s="69"/>
-      <c r="BJ10" s="69"/>
-      <c r="BK10" s="68">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="68"/>
-      <c r="BM10" s="68"/>
-      <c r="BN10" s="68"/>
-      <c r="BO10" s="68"/>
-      <c r="BP10" s="68"/>
-      <c r="BQ10" s="68"/>
+      <c r="BE10" s="71"/>
+      <c r="BF10" s="71"/>
+      <c r="BG10" s="71"/>
+      <c r="BH10" s="71"/>
+      <c r="BI10" s="71"/>
+      <c r="BJ10" s="71"/>
+      <c r="BK10" s="72">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="72"/>
+      <c r="BM10" s="72"/>
+      <c r="BN10" s="72"/>
+      <c r="BO10" s="72"/>
+      <c r="BP10" s="72"/>
+      <c r="BQ10" s="72"/>
       <c r="BR10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BS10" s="69" t="s">
+      <c r="BS10" s="71" t="s">
         <v>514</v>
       </c>
-      <c r="BT10" s="69"/>
-      <c r="BU10" s="69"/>
-      <c r="BV10" s="69"/>
-      <c r="BW10" s="69"/>
-      <c r="BX10" s="69"/>
-      <c r="BY10" s="69"/>
+      <c r="BT10" s="71"/>
+      <c r="BU10" s="71"/>
+      <c r="BV10" s="71"/>
+      <c r="BW10" s="71"/>
+      <c r="BX10" s="71"/>
+      <c r="BY10" s="71"/>
       <c r="BZ10" s="56">
         <v>0</v>
       </c>
@@ -9203,17 +9600,356 @@
       <c r="DR10" s="13" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="11" spans="1:122">
+      <c r="EN10" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EP10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EQ10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="ER10" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="ET10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EU10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EV10" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EX10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="EY10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="EZ10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FB10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FE10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FF10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FG10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FI10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FJ10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FK10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FL10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FM10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FN10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FO10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FP10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FQ10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FR10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FS10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FU10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FV10" s="1">
+        <v>0</v>
+      </c>
+      <c r="FW10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FX10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="FY10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="FZ10" s="1">
+        <v>0</v>
+      </c>
+      <c r="GA10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GB10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GC10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="GE10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GF10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GG10" s="1">
+        <v>0</v>
+      </c>
+      <c r="GH10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GJ10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK10" s="1">
+        <v>0</v>
+      </c>
+      <c r="GL10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GN10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GO10" s="1">
+        <v>0</v>
+      </c>
+      <c r="GP10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GQ10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GR10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GS10" s="1">
+        <v>0</v>
+      </c>
+      <c r="GT10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GU10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GV10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW10" s="1">
+        <v>0</v>
+      </c>
+      <c r="GX10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GY10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GZ10" s="1">
+        <v>0</v>
+      </c>
+      <c r="HA10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HB10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="HC10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="HE10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HF10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="HG10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HH10" s="1">
+        <v>0</v>
+      </c>
+      <c r="HI10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HJ10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="HK10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HL10" s="1">
+        <v>0</v>
+      </c>
+      <c r="HM10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HN10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="HO10" s="1">
+        <v>0</v>
+      </c>
+      <c r="HP10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HQ10" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="HR10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HS10" s="1">
+        <v>0</v>
+      </c>
+      <c r="HT10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HU10" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="HV10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HW10" s="1">
+        <v>0</v>
+      </c>
+      <c r="HX10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="HY10" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="HZ10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="IA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="IB10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="IC10" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="ID10" s="45">
+        <v>0</v>
+      </c>
+      <c r="IE10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IF10" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="IG10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IH10" s="45">
+        <v>0</v>
+      </c>
+      <c r="II10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IJ10" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="IK10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IL10" s="45">
+        <v>0</v>
+      </c>
+      <c r="IM10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IN10" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="IO10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IP10" s="45">
+        <v>0</v>
+      </c>
+      <c r="IQ10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="IR10" s="45" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="11" spans="1:252">
       <c r="A11" s="2"/>
-    </row>
-    <row r="14" spans="1:122">
+      <c r="B11" s="75" t="s">
+        <v>520</v>
+      </c>
+      <c r="EN11" s="1">
+        <v>0</v>
+      </c>
+      <c r="GV11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="GW11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:252">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:122">
+    <row r="15" spans="1:252">
       <c r="B15" s="2"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
       <c r="H15"/>
     </row>
     <row r="32" spans="1:1">
@@ -9230,20 +9966,38 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="DD5:DR5"/>
-    <mergeCell ref="DD8:DJ8"/>
-    <mergeCell ref="DL8:DR8"/>
-    <mergeCell ref="DD9:DF9"/>
-    <mergeCell ref="DH9:DJ9"/>
-    <mergeCell ref="DL9:DN9"/>
-    <mergeCell ref="DP9:DR9"/>
-    <mergeCell ref="CO5:DC5"/>
-    <mergeCell ref="CO8:CU8"/>
-    <mergeCell ref="CW8:DC8"/>
-    <mergeCell ref="CO9:CQ9"/>
-    <mergeCell ref="CS9:CU9"/>
-    <mergeCell ref="CW9:CY9"/>
-    <mergeCell ref="DA9:DC9"/>
+    <mergeCell ref="AG5:AU5"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="K8:Q8"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C5:Q5"/>
+    <mergeCell ref="R5:AF5"/>
+    <mergeCell ref="R8:X8"/>
+    <mergeCell ref="Z8:AF8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="AG8:AM8"/>
+    <mergeCell ref="AO8:AU8"/>
+    <mergeCell ref="AG9:AI9"/>
+    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="AO9:AQ9"/>
+    <mergeCell ref="AS9:AU9"/>
+    <mergeCell ref="AV5:BJ5"/>
+    <mergeCell ref="AV9:AX9"/>
+    <mergeCell ref="AZ9:BB9"/>
+    <mergeCell ref="BD9:BF9"/>
+    <mergeCell ref="BH9:BJ9"/>
+    <mergeCell ref="AV10:BB10"/>
+    <mergeCell ref="BD10:BJ10"/>
+    <mergeCell ref="BK9:BM9"/>
+    <mergeCell ref="BO9:BQ9"/>
+    <mergeCell ref="BS9:BU9"/>
     <mergeCell ref="BW9:BY9"/>
     <mergeCell ref="BK10:BQ10"/>
     <mergeCell ref="BS10:BY10"/>
@@ -9254,42 +10008,24 @@
     <mergeCell ref="CD9:CF9"/>
     <mergeCell ref="CH9:CJ9"/>
     <mergeCell ref="CL9:CN9"/>
-    <mergeCell ref="AV10:BB10"/>
-    <mergeCell ref="BD10:BJ10"/>
-    <mergeCell ref="BK9:BM9"/>
-    <mergeCell ref="BO9:BQ9"/>
-    <mergeCell ref="BS9:BU9"/>
     <mergeCell ref="BK5:BY5"/>
-    <mergeCell ref="AV5:BJ5"/>
-    <mergeCell ref="AV9:AX9"/>
-    <mergeCell ref="AZ9:BB9"/>
-    <mergeCell ref="BD9:BF9"/>
-    <mergeCell ref="BH9:BJ9"/>
-    <mergeCell ref="AG8:AM8"/>
-    <mergeCell ref="AO8:AU8"/>
-    <mergeCell ref="AG9:AI9"/>
-    <mergeCell ref="AK9:AM9"/>
-    <mergeCell ref="AO9:AQ9"/>
-    <mergeCell ref="AS9:AU9"/>
-    <mergeCell ref="C5:Q5"/>
-    <mergeCell ref="R5:AF5"/>
-    <mergeCell ref="R8:X8"/>
-    <mergeCell ref="Z8:AF8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="Z9:AB9"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AG5:AU5"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="K8:Q8"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="CO5:DC5"/>
+    <mergeCell ref="CO8:CU8"/>
+    <mergeCell ref="CW8:DC8"/>
+    <mergeCell ref="CO9:CQ9"/>
+    <mergeCell ref="CS9:CU9"/>
+    <mergeCell ref="CW9:CY9"/>
+    <mergeCell ref="DA9:DC9"/>
+    <mergeCell ref="DD5:DR5"/>
+    <mergeCell ref="DD8:DJ8"/>
+    <mergeCell ref="DL8:DR8"/>
+    <mergeCell ref="DD9:DF9"/>
+    <mergeCell ref="DH9:DJ9"/>
+    <mergeCell ref="DL9:DN9"/>
+    <mergeCell ref="DP9:DR9"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="C8:C9 J8:K9 F9:G9 N9:O9 U9:V9 AC9:AD9 AG8:AG9 AJ9:AK9 AR9:AS9 AY9:AZ9 BC9:BD10 BG9:BH9 BN9:BO9 BR9:BS10 BV9:BW9 BZ8:BZ9 CG8:CH9 CC9:CD9 CK9:CL9 CO8:CO9 CV8:CW9 CR9:CS9 CZ9:DA9 DS8:XFD10 DD8:DD9 DK8:DL9 DG9:DH9 BZ10:DR10 R8:R9 AV9 C10:AV10 BK9:BK10 AV8:BY8 C11:XFD1048576 Y8:Z9 AN8:AO9 DO9:DP9">
+  <conditionalFormatting sqref="AV8:BY8 C8:C9 J8:K9 R8:R9 Y8:Z9 AG8:AG9 AN8:AO9 BZ8:BZ9 CG8:CH9 CO8:CO9 CV8:CW9 DD8:DD9 DK8:DL9 F9:G9 N9:O9 U9:V9 AC9:AD9 AJ9:AK9 AR9:AS9 AV9 AY9:AZ9 BG9:BH9 BN9:BO9 BV9:BW9 CC9:CD9 CK9:CL9 CR9:CS9 CZ9:DA9 DG9:DH9 DO9:DP9 BC9:BD10 BK9:BK10 BR9:BS10 C10:AV10 C11:XFD1048576 BZ10:EU10 DS8:EU9 EV8:IC10 IS8:XFD10">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C8&lt;&gt;""</formula>
     </cfRule>

</xml_diff>

<commit_message>
edit behaviormodel and timingchart
</commit_message>
<xml_diff>
--- a/project/nystromformer_timingchart.xlsx
+++ b/project/nystromformer_timingchart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/furuta/LALSIE/GPT/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2065AF81-7E05-6444-A6E1-D8AD58973475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDBF476-F7C8-1A47-8C3F-74DDC388297A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="920" windowWidth="14480" windowHeight="18060" firstSheet="3" activeTab="6" xr2:uid="{71DF794F-EDEF-1649-A071-280480E3C700}"/>
+    <workbookView xWindow="14780" yWindow="920" windowWidth="14460" windowHeight="18040" firstSheet="3" activeTab="6" xr2:uid="{71DF794F-EDEF-1649-A071-280480E3C700}"/>
   </bookViews>
   <sheets>
     <sheet name="timing_chart" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="527">
   <si>
     <t>Query</t>
     <phoneticPr fontId="1"/>
@@ -2156,12 +2156,20 @@
     <t>k3 * v</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>63 (n/m-1)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V &lt;- matmul_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2272,8 +2280,25 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2358,8 +2383,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -2512,13 +2561,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2687,65 +2831,197 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7976,10 +8252,10 @@
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="61" t="s">
+      <c r="F16" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="61"/>
+      <c r="G16" s="57"/>
       <c r="H16"/>
     </row>
     <row r="17" spans="1:51">
@@ -8267,1689 +8543,2411 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120B20A9-82A7-4D47-8C93-28558266A36A}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:IR35"/>
+  <dimension ref="A1:IU35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="50" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:252">
+    <row r="1" spans="1:255">
       <c r="A1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:252">
+    <row r="2" spans="1:255">
       <c r="A2" s="55" t="s">
         <v>487</v>
       </c>
       <c r="B2" s="55"/>
     </row>
-    <row r="3" spans="1:252">
+    <row r="3" spans="1:255" s="87" customFormat="1">
       <c r="A3" s="55" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="4" spans="1:252" ht="21" customHeight="1">
+      <c r="B3"/>
+      <c r="Q3" s="118">
+        <v>16777216</v>
+      </c>
+      <c r="AF3" s="118">
+        <v>33554432</v>
+      </c>
+      <c r="AU3" s="118">
+        <v>50331648</v>
+      </c>
+      <c r="BJ3" s="118">
+        <v>50397184</v>
+      </c>
+      <c r="BY3" s="118">
+        <v>50462720</v>
+      </c>
+      <c r="CN3" s="118">
+        <v>50724864</v>
+      </c>
+      <c r="DC3" s="118">
+        <v>50728960</v>
+      </c>
+      <c r="DR3" s="118">
+        <v>50991104</v>
+      </c>
+      <c r="EI3" s="118">
+        <v>50991140</v>
+      </c>
+      <c r="HB3" s="118">
+        <v>50992772</v>
+      </c>
+      <c r="HQ3" s="118">
+        <v>50996868</v>
+      </c>
+      <c r="IF3" s="118">
+        <v>51259012</v>
+      </c>
+      <c r="IU3" s="118">
+        <v>51521156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:255" s="87" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A4" s="55" t="s">
         <v>489</v>
       </c>
       <c r="B4" s="55" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="5" spans="1:252" s="60" customFormat="1" ht="21" customHeight="1">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59" t="s">
+      <c r="C4" s="87">
+        <v>1</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="87">
+        <v>256</v>
+      </c>
+      <c r="F4" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="118">
+        <v>65536</v>
+      </c>
+      <c r="Q4" s="118">
+        <v>16777216</v>
+      </c>
+      <c r="AF4" s="118">
+        <v>16777216</v>
+      </c>
+      <c r="AU4" s="118">
+        <v>16777216</v>
+      </c>
+      <c r="AV4" s="87">
+        <v>1</v>
+      </c>
+      <c r="BB4" s="87">
+        <v>16320</v>
+      </c>
+      <c r="BJ4" s="118">
+        <v>65536</v>
+      </c>
+      <c r="BY4" s="118">
+        <v>65536</v>
+      </c>
+      <c r="BZ4" s="87">
+        <v>1</v>
+      </c>
+      <c r="CF4" s="87">
+        <v>1024</v>
+      </c>
+      <c r="CN4" s="118">
+        <v>262144</v>
+      </c>
+      <c r="CO4" s="87">
+        <v>1</v>
+      </c>
+      <c r="CU4" s="87">
+        <v>1024</v>
+      </c>
+      <c r="DC4" s="118">
+        <v>4096</v>
+      </c>
+      <c r="DD4" s="87">
+        <v>1</v>
+      </c>
+      <c r="DJ4" s="118">
+        <v>65536</v>
+      </c>
+      <c r="DR4" s="118">
+        <v>262144</v>
+      </c>
+      <c r="DS4" s="87">
+        <v>1</v>
+      </c>
+      <c r="DY4" s="87">
+        <v>16</v>
+      </c>
+      <c r="EB4" s="87">
+        <v>20</v>
+      </c>
+      <c r="EI4" s="87">
+        <v>36</v>
+      </c>
+      <c r="EJ4" s="87">
+        <v>1</v>
+      </c>
+      <c r="EP4" s="87">
+        <v>16</v>
+      </c>
+      <c r="EX4" s="87">
+        <v>64</v>
+      </c>
+      <c r="EY4" s="87">
+        <v>1</v>
+      </c>
+      <c r="FM4" s="87">
+        <v>64</v>
+      </c>
+      <c r="FN4" s="87">
+        <v>1</v>
+      </c>
+      <c r="GB4" s="87">
+        <v>64</v>
+      </c>
+      <c r="GC4" s="87">
+        <v>1</v>
+      </c>
+      <c r="GQ4" s="87">
+        <v>64</v>
+      </c>
+      <c r="GX4" s="87">
+        <v>60</v>
+      </c>
+      <c r="HB4" s="118">
+        <v>1632</v>
+      </c>
+      <c r="HC4" s="87">
+        <v>1</v>
+      </c>
+      <c r="HI4" s="87">
+        <v>16</v>
+      </c>
+      <c r="HQ4" s="118">
+        <v>4096</v>
+      </c>
+      <c r="HR4" s="87">
+        <v>1</v>
+      </c>
+      <c r="HX4" s="118">
+        <v>65536</v>
+      </c>
+      <c r="IF4" s="118">
+        <v>262144</v>
+      </c>
+      <c r="IG4" s="87">
+        <v>1</v>
+      </c>
+      <c r="IM4" s="118">
+        <v>1024</v>
+      </c>
+      <c r="IU4" s="118">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:255" s="63" customFormat="1" ht="21" customHeight="1" thickBot="1">
+      <c r="A5" s="58"/>
+      <c r="B5" s="58" t="s">
         <v>462</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="119" t="s">
         <v>507</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74" t="s">
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59" t="s">
         <v>508</v>
       </c>
-      <c r="S5" s="74"/>
-      <c r="T5" s="74"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74"/>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="74"/>
-      <c r="AA5" s="74"/>
-      <c r="AB5" s="74"/>
-      <c r="AC5" s="74"/>
-      <c r="AD5" s="74"/>
-      <c r="AE5" s="74"/>
-      <c r="AF5" s="74"/>
-      <c r="AG5" s="74" t="s">
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
+      <c r="AC5" s="59"/>
+      <c r="AD5" s="59"/>
+      <c r="AE5" s="59"/>
+      <c r="AF5" s="59"/>
+      <c r="AG5" s="59" t="s">
         <v>509</v>
       </c>
-      <c r="AH5" s="74"/>
-      <c r="AI5" s="74"/>
-      <c r="AJ5" s="74"/>
-      <c r="AK5" s="74"/>
-      <c r="AL5" s="74"/>
-      <c r="AM5" s="74"/>
-      <c r="AN5" s="74"/>
-      <c r="AO5" s="74"/>
-      <c r="AP5" s="74"/>
-      <c r="AQ5" s="74"/>
-      <c r="AR5" s="74"/>
-      <c r="AS5" s="74"/>
-      <c r="AT5" s="74"/>
-      <c r="AU5" s="74"/>
-      <c r="AV5" s="73" t="s">
+      <c r="AH5" s="59"/>
+      <c r="AI5" s="59"/>
+      <c r="AJ5" s="59"/>
+      <c r="AK5" s="59"/>
+      <c r="AL5" s="59"/>
+      <c r="AM5" s="59"/>
+      <c r="AN5" s="59"/>
+      <c r="AO5" s="59"/>
+      <c r="AP5" s="59"/>
+      <c r="AQ5" s="59"/>
+      <c r="AR5" s="59"/>
+      <c r="AS5" s="59"/>
+      <c r="AT5" s="59"/>
+      <c r="AU5" s="59"/>
+      <c r="AV5" s="60" t="s">
         <v>510</v>
       </c>
-      <c r="AW5" s="73"/>
-      <c r="AX5" s="73"/>
-      <c r="AY5" s="73"/>
-      <c r="AZ5" s="73"/>
-      <c r="BA5" s="73"/>
-      <c r="BB5" s="73"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="73"/>
-      <c r="BE5" s="73"/>
-      <c r="BF5" s="73"/>
-      <c r="BG5" s="73"/>
-      <c r="BH5" s="73"/>
-      <c r="BI5" s="73"/>
-      <c r="BJ5" s="73"/>
-      <c r="BK5" s="73" t="s">
+      <c r="AW5" s="60"/>
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="60"/>
+      <c r="AZ5" s="60"/>
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
+      <c r="BC5" s="60"/>
+      <c r="BD5" s="60"/>
+      <c r="BE5" s="60"/>
+      <c r="BF5" s="60"/>
+      <c r="BG5" s="60"/>
+      <c r="BH5" s="60"/>
+      <c r="BI5" s="60"/>
+      <c r="BJ5" s="60"/>
+      <c r="BK5" s="60" t="s">
         <v>511</v>
       </c>
-      <c r="BL5" s="73"/>
-      <c r="BM5" s="73"/>
-      <c r="BN5" s="73"/>
-      <c r="BO5" s="73"/>
-      <c r="BP5" s="73"/>
-      <c r="BQ5" s="73"/>
-      <c r="BR5" s="73"/>
-      <c r="BS5" s="73"/>
-      <c r="BT5" s="73"/>
-      <c r="BU5" s="73"/>
-      <c r="BV5" s="73"/>
-      <c r="BW5" s="73"/>
-      <c r="BX5" s="73"/>
-      <c r="BY5" s="73"/>
-      <c r="BZ5" s="62" t="s">
+      <c r="BL5" s="60"/>
+      <c r="BM5" s="60"/>
+      <c r="BN5" s="60"/>
+      <c r="BO5" s="60"/>
+      <c r="BP5" s="60"/>
+      <c r="BQ5" s="60"/>
+      <c r="BR5" s="60"/>
+      <c r="BS5" s="60"/>
+      <c r="BT5" s="60"/>
+      <c r="BU5" s="60"/>
+      <c r="BV5" s="60"/>
+      <c r="BW5" s="60"/>
+      <c r="BX5" s="60"/>
+      <c r="BY5" s="60"/>
+      <c r="BZ5" s="61" t="s">
         <v>513</v>
       </c>
-      <c r="CA5" s="62"/>
-      <c r="CB5" s="62"/>
-      <c r="CC5" s="62"/>
-      <c r="CD5" s="62"/>
-      <c r="CE5" s="62"/>
-      <c r="CF5" s="62"/>
-      <c r="CG5" s="62"/>
-      <c r="CH5" s="62"/>
-      <c r="CI5" s="62"/>
-      <c r="CJ5" s="62"/>
-      <c r="CK5" s="62"/>
-      <c r="CL5" s="62"/>
-      <c r="CM5" s="62"/>
-      <c r="CN5" s="62"/>
-      <c r="CO5" s="62" t="s">
+      <c r="CA5" s="61"/>
+      <c r="CB5" s="61"/>
+      <c r="CC5" s="61"/>
+      <c r="CD5" s="61"/>
+      <c r="CE5" s="61"/>
+      <c r="CF5" s="61"/>
+      <c r="CG5" s="61"/>
+      <c r="CH5" s="61"/>
+      <c r="CI5" s="61"/>
+      <c r="CJ5" s="61"/>
+      <c r="CK5" s="61"/>
+      <c r="CL5" s="61"/>
+      <c r="CM5" s="61"/>
+      <c r="CN5" s="61"/>
+      <c r="CO5" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="CP5" s="62"/>
-      <c r="CQ5" s="62"/>
-      <c r="CR5" s="62"/>
-      <c r="CS5" s="62"/>
-      <c r="CT5" s="62"/>
-      <c r="CU5" s="62"/>
-      <c r="CV5" s="62"/>
-      <c r="CW5" s="62"/>
-      <c r="CX5" s="62"/>
-      <c r="CY5" s="62"/>
-      <c r="CZ5" s="62"/>
-      <c r="DA5" s="62"/>
-      <c r="DB5" s="62"/>
-      <c r="DC5" s="62"/>
-      <c r="DD5" s="62" t="s">
+      <c r="CP5" s="61"/>
+      <c r="CQ5" s="61"/>
+      <c r="CR5" s="61"/>
+      <c r="CS5" s="61"/>
+      <c r="CT5" s="61"/>
+      <c r="CU5" s="61"/>
+      <c r="CV5" s="61"/>
+      <c r="CW5" s="61"/>
+      <c r="CX5" s="61"/>
+      <c r="CY5" s="61"/>
+      <c r="CZ5" s="61"/>
+      <c r="DA5" s="61"/>
+      <c r="DB5" s="61"/>
+      <c r="DC5" s="61"/>
+      <c r="DD5" s="61" t="s">
         <v>516</v>
       </c>
-      <c r="DE5" s="62"/>
-      <c r="DF5" s="62"/>
-      <c r="DG5" s="62"/>
-      <c r="DH5" s="62"/>
-      <c r="DI5" s="62"/>
-      <c r="DJ5" s="62"/>
-      <c r="DK5" s="62"/>
-      <c r="DL5" s="62"/>
-      <c r="DM5" s="62"/>
-      <c r="DN5" s="62"/>
-      <c r="DO5" s="62"/>
-      <c r="DP5" s="62"/>
-      <c r="DQ5" s="62"/>
-      <c r="DR5" s="62"/>
-      <c r="DS5" s="60" t="s">
+      <c r="DE5" s="61"/>
+      <c r="DF5" s="61"/>
+      <c r="DG5" s="61"/>
+      <c r="DH5" s="61"/>
+      <c r="DI5" s="61"/>
+      <c r="DJ5" s="61"/>
+      <c r="DK5" s="61"/>
+      <c r="DL5" s="61"/>
+      <c r="DM5" s="61"/>
+      <c r="DN5" s="61"/>
+      <c r="DO5" s="61"/>
+      <c r="DP5" s="61"/>
+      <c r="DQ5" s="61"/>
+      <c r="DR5" s="61"/>
+      <c r="DS5" s="62" t="s">
         <v>518</v>
       </c>
-      <c r="EN5" s="60" t="s">
+      <c r="DT5" s="62"/>
+      <c r="DU5" s="62"/>
+      <c r="DV5" s="62"/>
+      <c r="DW5" s="62"/>
+      <c r="DX5" s="62"/>
+      <c r="DY5" s="62"/>
+      <c r="DZ5" s="62"/>
+      <c r="EA5" s="62"/>
+      <c r="EB5" s="62"/>
+      <c r="EC5" s="62"/>
+      <c r="ED5" s="62"/>
+      <c r="EE5" s="62"/>
+      <c r="EF5" s="62"/>
+      <c r="EG5" s="62"/>
+      <c r="EH5" s="62"/>
+      <c r="EI5" s="62"/>
+      <c r="EJ5" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="FC5" s="60" t="s">
+      <c r="EK5" s="62"/>
+      <c r="EL5" s="62"/>
+      <c r="EM5" s="62"/>
+      <c r="EN5" s="62"/>
+      <c r="EO5" s="62"/>
+      <c r="EP5" s="62"/>
+      <c r="EQ5" s="62"/>
+      <c r="ER5" s="62"/>
+      <c r="ES5" s="62"/>
+      <c r="ET5" s="62"/>
+      <c r="EU5" s="62"/>
+      <c r="EV5" s="62"/>
+      <c r="EW5" s="62"/>
+      <c r="EX5" s="62"/>
+      <c r="EY5" s="62" t="s">
         <v>404</v>
       </c>
-      <c r="FR5" s="60" t="s">
+      <c r="EZ5" s="62"/>
+      <c r="FA5" s="62"/>
+      <c r="FB5" s="62"/>
+      <c r="FC5" s="62"/>
+      <c r="FD5" s="62"/>
+      <c r="FE5" s="62"/>
+      <c r="FF5" s="62"/>
+      <c r="FG5" s="62"/>
+      <c r="FH5" s="62"/>
+      <c r="FI5" s="62"/>
+      <c r="FJ5" s="62"/>
+      <c r="FK5" s="62"/>
+      <c r="FL5" s="62"/>
+      <c r="FM5" s="62"/>
+      <c r="FN5" s="62" t="s">
         <v>410</v>
       </c>
-      <c r="GG5" s="60" t="s">
+      <c r="FO5" s="62"/>
+      <c r="FP5" s="62"/>
+      <c r="FQ5" s="62"/>
+      <c r="FR5" s="62"/>
+      <c r="FS5" s="62"/>
+      <c r="FT5" s="62"/>
+      <c r="FU5" s="62"/>
+      <c r="FV5" s="62"/>
+      <c r="FW5" s="62"/>
+      <c r="FX5" s="62"/>
+      <c r="FY5" s="62"/>
+      <c r="FZ5" s="62"/>
+      <c r="GA5" s="62"/>
+      <c r="GB5" s="62"/>
+      <c r="GC5" s="62" t="s">
         <v>521</v>
       </c>
-      <c r="GZ5" s="60" t="s">
+      <c r="GD5" s="62"/>
+      <c r="GE5" s="62"/>
+      <c r="GF5" s="62"/>
+      <c r="GG5" s="62"/>
+      <c r="GH5" s="62"/>
+      <c r="GI5" s="62"/>
+      <c r="GJ5" s="62"/>
+      <c r="GK5" s="62"/>
+      <c r="GL5" s="62"/>
+      <c r="GM5" s="62"/>
+      <c r="GN5" s="62"/>
+      <c r="GO5" s="62"/>
+      <c r="GP5" s="62"/>
+      <c r="GQ5" s="62"/>
+      <c r="GR5" s="115" t="s">
+        <v>526</v>
+      </c>
+      <c r="GS5" s="116"/>
+      <c r="GT5" s="116"/>
+      <c r="GU5" s="116"/>
+      <c r="GV5" s="116"/>
+      <c r="GW5" s="116"/>
+      <c r="GX5" s="117"/>
+      <c r="GY5" s="62"/>
+      <c r="GZ5" s="62"/>
+      <c r="HA5" s="62"/>
+      <c r="HB5" s="62"/>
+      <c r="HC5" s="61" t="s">
         <v>522</v>
       </c>
-      <c r="HO5" s="60" t="s">
+      <c r="HD5" s="61"/>
+      <c r="HE5" s="61"/>
+      <c r="HF5" s="61"/>
+      <c r="HG5" s="61"/>
+      <c r="HH5" s="61"/>
+      <c r="HI5" s="61"/>
+      <c r="HJ5" s="61"/>
+      <c r="HK5" s="61"/>
+      <c r="HL5" s="61"/>
+      <c r="HM5" s="61"/>
+      <c r="HN5" s="61"/>
+      <c r="HO5" s="61"/>
+      <c r="HP5" s="61"/>
+      <c r="HQ5" s="61"/>
+      <c r="HR5" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="ID5" s="60" t="s">
+      <c r="HS5" s="61"/>
+      <c r="HT5" s="61"/>
+      <c r="HU5" s="61"/>
+      <c r="HV5" s="61"/>
+      <c r="HW5" s="61"/>
+      <c r="HX5" s="61"/>
+      <c r="HY5" s="61"/>
+      <c r="HZ5" s="61"/>
+      <c r="IA5" s="61"/>
+      <c r="IB5" s="61"/>
+      <c r="IC5" s="61"/>
+      <c r="ID5" s="61"/>
+      <c r="IE5" s="61"/>
+      <c r="IF5" s="61"/>
+      <c r="IG5" s="61" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:252" ht="21" customHeight="1">
+      <c r="IH5" s="61"/>
+      <c r="II5" s="61"/>
+      <c r="IJ5" s="61"/>
+      <c r="IK5" s="61"/>
+      <c r="IL5" s="61"/>
+      <c r="IM5" s="61"/>
+      <c r="IN5" s="61"/>
+      <c r="IO5" s="61"/>
+      <c r="IP5" s="61"/>
+      <c r="IQ5" s="61"/>
+      <c r="IR5" s="61"/>
+      <c r="IS5" s="61"/>
+      <c r="IT5" s="61"/>
+      <c r="IU5" s="61"/>
+    </row>
+    <row r="7" spans="1:255" ht="21" customHeight="1">
       <c r="A7" s="55"/>
       <c r="B7" s="55"/>
-    </row>
-    <row r="8" spans="1:252">
+      <c r="EB7" s="17"/>
+    </row>
+    <row r="8" spans="1:255">
       <c r="A8" s="55" t="s">
         <v>503</v>
       </c>
       <c r="B8" s="55" t="s">
         <v>504</v>
       </c>
-      <c r="C8" s="63">
-        <v>0</v>
-      </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="66" t="s">
+      <c r="C8" s="64">
+        <v>0</v>
+      </c>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="68" t="s">
         <v>517</v>
       </c>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="63">
-        <v>0</v>
-      </c>
-      <c r="S8" s="64"/>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="64"/>
-      <c r="X8" s="65"/>
-      <c r="Y8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z8" s="66" t="s">
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="64">
+        <v>0</v>
+      </c>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="65"/>
+      <c r="X8" s="66"/>
+      <c r="Y8" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z8" s="68" t="s">
         <v>517</v>
       </c>
-      <c r="AA8" s="67"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="68"/>
-      <c r="AG8" s="63">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="64"/>
-      <c r="AI8" s="64"/>
-      <c r="AJ8" s="64"/>
-      <c r="AK8" s="64"/>
-      <c r="AL8" s="64"/>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO8" s="66" t="s">
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="70"/>
+      <c r="AG8" s="64">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="65"/>
+      <c r="AI8" s="65"/>
+      <c r="AJ8" s="65"/>
+      <c r="AK8" s="65"/>
+      <c r="AL8" s="65"/>
+      <c r="AM8" s="66"/>
+      <c r="AN8" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO8" s="68" t="s">
         <v>517</v>
       </c>
-      <c r="AP8" s="67"/>
-      <c r="AQ8" s="67"/>
-      <c r="AR8" s="67"/>
-      <c r="AS8" s="67"/>
-      <c r="AT8" s="67"/>
-      <c r="AU8" s="68"/>
-      <c r="AV8" s="57">
-        <v>0</v>
-      </c>
-      <c r="AW8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AX8" s="58">
+      <c r="AP8" s="69"/>
+      <c r="AQ8" s="69"/>
+      <c r="AR8" s="69"/>
+      <c r="AS8" s="69"/>
+      <c r="AT8" s="69"/>
+      <c r="AU8" s="70"/>
+      <c r="AV8" s="71">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX8" s="73" t="s">
+        <v>525</v>
+      </c>
+      <c r="AY8" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ8" s="71">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB8" s="73" t="s">
+        <v>525</v>
+      </c>
+      <c r="BC8" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="BD8" s="71">
+        <v>192</v>
+      </c>
+      <c r="BE8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BF8" s="73">
+        <v>255</v>
+      </c>
+      <c r="BG8" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH8" s="71">
+        <v>192</v>
+      </c>
+      <c r="BI8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BJ8" s="73">
+        <v>255</v>
+      </c>
+      <c r="BK8" s="71">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BM8" s="73">
         <v>63</v>
       </c>
-      <c r="AY8" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="AZ8" s="57">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BB8" s="58">
+      <c r="BN8" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="BO8" s="71">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BQ8" s="73">
         <v>63</v>
       </c>
-      <c r="BC8" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="BD8" s="57">
+      <c r="BR8" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="BS8" s="71">
         <v>192</v>
       </c>
-      <c r="BE8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BF8" s="58">
+      <c r="BT8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BU8" s="73">
         <v>255</v>
       </c>
-      <c r="BG8" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="BH8" s="57">
+      <c r="BV8" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW8" s="71">
         <v>192</v>
       </c>
-      <c r="BI8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BJ8" s="58">
+      <c r="BX8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BY8" s="73">
         <v>255</v>
       </c>
-      <c r="BK8" s="57">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BM8" s="58">
-        <v>63</v>
-      </c>
-      <c r="BN8" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="BO8" s="57">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BQ8" s="58">
-        <v>63</v>
-      </c>
-      <c r="BR8" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="BS8" s="57">
-        <v>192</v>
-      </c>
-      <c r="BT8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BU8" s="58">
-        <v>255</v>
-      </c>
-      <c r="BV8" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW8" s="57">
-        <v>192</v>
-      </c>
-      <c r="BX8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BY8" s="58">
-        <v>255</v>
-      </c>
-      <c r="BZ8" s="63">
-        <v>0</v>
-      </c>
-      <c r="CA8" s="64"/>
-      <c r="CB8" s="64"/>
-      <c r="CC8" s="64"/>
-      <c r="CD8" s="64"/>
-      <c r="CE8" s="64"/>
-      <c r="CF8" s="65"/>
-      <c r="CG8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CH8" s="66" t="s">
+      <c r="BZ8" s="64">
+        <v>0</v>
+      </c>
+      <c r="CA8" s="65"/>
+      <c r="CB8" s="65"/>
+      <c r="CC8" s="65"/>
+      <c r="CD8" s="65"/>
+      <c r="CE8" s="65"/>
+      <c r="CF8" s="66"/>
+      <c r="CG8" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CH8" s="74" t="s">
         <v>517</v>
       </c>
-      <c r="CI8" s="67"/>
-      <c r="CJ8" s="67"/>
-      <c r="CK8" s="67"/>
-      <c r="CL8" s="67"/>
-      <c r="CM8" s="67"/>
-      <c r="CN8" s="68"/>
-      <c r="CO8" s="63">
-        <v>0</v>
-      </c>
-      <c r="CP8" s="64"/>
-      <c r="CQ8" s="64"/>
-      <c r="CR8" s="64"/>
-      <c r="CS8" s="64"/>
-      <c r="CT8" s="64"/>
-      <c r="CU8" s="65"/>
-      <c r="CV8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CW8" s="66" t="s">
+      <c r="CI8" s="75"/>
+      <c r="CJ8" s="75"/>
+      <c r="CK8" s="75"/>
+      <c r="CL8" s="75"/>
+      <c r="CM8" s="75"/>
+      <c r="CN8" s="76"/>
+      <c r="CO8" s="64">
+        <v>0</v>
+      </c>
+      <c r="CP8" s="65"/>
+      <c r="CQ8" s="65"/>
+      <c r="CR8" s="65"/>
+      <c r="CS8" s="65"/>
+      <c r="CT8" s="65"/>
+      <c r="CU8" s="66"/>
+      <c r="CV8" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CW8" s="74" t="s">
         <v>514</v>
       </c>
-      <c r="CX8" s="67"/>
-      <c r="CY8" s="67"/>
-      <c r="CZ8" s="67"/>
-      <c r="DA8" s="67"/>
-      <c r="DB8" s="67"/>
-      <c r="DC8" s="68"/>
-      <c r="DD8" s="63">
-        <v>0</v>
-      </c>
-      <c r="DE8" s="64"/>
-      <c r="DF8" s="64"/>
-      <c r="DG8" s="64"/>
-      <c r="DH8" s="64"/>
-      <c r="DI8" s="64"/>
-      <c r="DJ8" s="65"/>
-      <c r="DK8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DL8" s="66" t="s">
+      <c r="CX8" s="75"/>
+      <c r="CY8" s="75"/>
+      <c r="CZ8" s="75"/>
+      <c r="DA8" s="75"/>
+      <c r="DB8" s="75"/>
+      <c r="DC8" s="76"/>
+      <c r="DD8" s="64">
+        <v>0</v>
+      </c>
+      <c r="DE8" s="65"/>
+      <c r="DF8" s="65"/>
+      <c r="DG8" s="65"/>
+      <c r="DH8" s="65"/>
+      <c r="DI8" s="65"/>
+      <c r="DJ8" s="66"/>
+      <c r="DK8" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DL8" s="74" t="s">
         <v>514</v>
       </c>
-      <c r="DM8" s="67"/>
-      <c r="DN8" s="67"/>
-      <c r="DO8" s="67"/>
-      <c r="DP8" s="67"/>
-      <c r="DQ8" s="67"/>
-      <c r="DR8" s="68"/>
-      <c r="DS8" s="1">
-        <v>0</v>
-      </c>
-      <c r="DV8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DW8" s="1" t="s">
+      <c r="DM8" s="75"/>
+      <c r="DN8" s="75"/>
+      <c r="DO8" s="75"/>
+      <c r="DP8" s="75"/>
+      <c r="DQ8" s="75"/>
+      <c r="DR8" s="75"/>
+      <c r="DS8" s="77">
+        <v>0</v>
+      </c>
+      <c r="DT8" s="77"/>
+      <c r="DU8" s="77"/>
+      <c r="DV8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="DW8" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="DZ8" s="1">
-        <v>0</v>
-      </c>
-      <c r="EC8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ED8" s="1" t="s">
+      <c r="DX8" s="78"/>
+      <c r="DY8" s="74"/>
+      <c r="DZ8" s="111">
+        <v>0</v>
+      </c>
+      <c r="EA8" s="112" t="s">
+        <v>11</v>
+      </c>
+      <c r="EB8" s="113" t="s">
         <v>514</v>
       </c>
-      <c r="EG8" s="1">
-        <v>0</v>
-      </c>
-      <c r="EJ8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EK8" s="1" t="s">
+      <c r="EC8" s="66">
+        <v>0</v>
+      </c>
+      <c r="ED8" s="77"/>
+      <c r="EE8" s="77"/>
+      <c r="EF8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="EG8" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="EN8" s="1">
-        <v>0</v>
-      </c>
-      <c r="EU8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EV8" s="1" t="s">
+      <c r="EH8" s="78"/>
+      <c r="EI8" s="78"/>
+      <c r="EJ8" s="79">
+        <v>0</v>
+      </c>
+      <c r="EK8" s="80"/>
+      <c r="EL8" s="80"/>
+      <c r="EM8" s="80"/>
+      <c r="EN8" s="80"/>
+      <c r="EO8" s="80"/>
+      <c r="EP8" s="81"/>
+      <c r="EQ8" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="ER8" s="83" t="s">
+        <v>519</v>
+      </c>
+      <c r="ES8" s="84"/>
+      <c r="ET8" s="84"/>
+      <c r="EU8" s="84"/>
+      <c r="EV8" s="84"/>
+      <c r="EW8" s="84"/>
+      <c r="EX8" s="85"/>
+      <c r="EY8" s="86">
+        <v>0</v>
+      </c>
+      <c r="EZ8" s="86"/>
+      <c r="FA8" s="86"/>
+      <c r="FB8" s="86"/>
+      <c r="FC8" s="86"/>
+      <c r="FD8" s="86"/>
+      <c r="FE8" s="86"/>
+      <c r="FF8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FG8" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="FC8" s="1">
-        <v>0</v>
-      </c>
-      <c r="FJ8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FK8" s="1" t="s">
+      <c r="FH8" s="78"/>
+      <c r="FI8" s="78"/>
+      <c r="FJ8" s="78"/>
+      <c r="FK8" s="78"/>
+      <c r="FL8" s="78"/>
+      <c r="FM8" s="78"/>
+      <c r="FN8" s="86">
+        <v>0</v>
+      </c>
+      <c r="FO8" s="86"/>
+      <c r="FP8" s="86"/>
+      <c r="FQ8" s="86"/>
+      <c r="FR8" s="86"/>
+      <c r="FS8" s="86"/>
+      <c r="FT8" s="86"/>
+      <c r="FU8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FV8" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="FR8" s="1">
-        <v>0</v>
-      </c>
-      <c r="FY8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FZ8" s="1" t="s">
+      <c r="FW8" s="78"/>
+      <c r="FX8" s="78"/>
+      <c r="FY8" s="78"/>
+      <c r="FZ8" s="78"/>
+      <c r="GA8" s="78"/>
+      <c r="GB8" s="78"/>
+      <c r="GC8" s="86">
+        <v>0</v>
+      </c>
+      <c r="GD8" s="86"/>
+      <c r="GE8" s="86"/>
+      <c r="GF8" s="86"/>
+      <c r="GG8" s="86"/>
+      <c r="GH8" s="86"/>
+      <c r="GI8" s="86"/>
+      <c r="GJ8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK8" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="GG8" s="1">
-        <v>0</v>
-      </c>
-      <c r="GN8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GO8" s="1" t="s">
+      <c r="GL8" s="78"/>
+      <c r="GM8" s="78"/>
+      <c r="GN8" s="78"/>
+      <c r="GO8" s="78"/>
+      <c r="GP8" s="78"/>
+      <c r="GQ8" s="78"/>
+      <c r="GR8" s="64">
+        <v>0</v>
+      </c>
+      <c r="GS8" s="65"/>
+      <c r="GT8" s="66"/>
+      <c r="GU8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV8" s="74" t="s">
         <v>514</v>
       </c>
-      <c r="GV8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GW8" s="1">
-        <v>0</v>
-      </c>
-      <c r="GX8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GY8" s="1" t="s">
+      <c r="GW8" s="75"/>
+      <c r="GX8" s="76"/>
+      <c r="GY8" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="GZ8" s="88">
+        <v>0</v>
+      </c>
+      <c r="HA8" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="HB8" s="89" t="s">
         <v>514</v>
       </c>
-      <c r="GZ8" s="1">
-        <v>0</v>
-      </c>
-      <c r="HG8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HH8" s="1" t="s">
+      <c r="HC8" s="77">
+        <v>0</v>
+      </c>
+      <c r="HD8" s="77"/>
+      <c r="HE8" s="77"/>
+      <c r="HF8" s="77"/>
+      <c r="HG8" s="77"/>
+      <c r="HH8" s="77"/>
+      <c r="HI8" s="77"/>
+      <c r="HJ8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HK8" s="78" t="s">
         <v>517</v>
       </c>
-      <c r="HO8" s="1">
-        <v>0</v>
-      </c>
-      <c r="HV8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HW8" s="1" t="s">
+      <c r="HL8" s="78"/>
+      <c r="HM8" s="78"/>
+      <c r="HN8" s="78"/>
+      <c r="HO8" s="78"/>
+      <c r="HP8" s="78"/>
+      <c r="HQ8" s="78"/>
+      <c r="HR8" s="77">
+        <v>0</v>
+      </c>
+      <c r="HS8" s="77"/>
+      <c r="HT8" s="77"/>
+      <c r="HU8" s="77"/>
+      <c r="HV8" s="77"/>
+      <c r="HW8" s="77"/>
+      <c r="HX8" s="77"/>
+      <c r="HY8" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HZ8" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="ID8" s="45">
-        <v>0</v>
-      </c>
-      <c r="IE8" s="46"/>
-      <c r="IF8" s="46"/>
-      <c r="IG8" s="46"/>
-      <c r="IH8" s="46"/>
-      <c r="II8" s="46"/>
-      <c r="IJ8" s="46"/>
-      <c r="IK8" s="45" t="s">
+      <c r="IA8" s="78"/>
+      <c r="IB8" s="78"/>
+      <c r="IC8" s="78"/>
+      <c r="ID8" s="78"/>
+      <c r="IE8" s="78"/>
+      <c r="IF8" s="78"/>
+      <c r="IG8" s="90">
+        <v>0</v>
+      </c>
+      <c r="IH8" s="90"/>
+      <c r="II8" s="90"/>
+      <c r="IJ8" s="90"/>
+      <c r="IK8" s="90"/>
+      <c r="IL8" s="90"/>
+      <c r="IM8" s="90"/>
+      <c r="IN8" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="IL8" s="45" t="s">
+      <c r="IO8" s="92" t="s">
         <v>523</v>
       </c>
-      <c r="IM8" s="46"/>
-      <c r="IN8" s="46"/>
-      <c r="IO8" s="46"/>
-      <c r="IP8" s="46"/>
-      <c r="IQ8" s="46"/>
-      <c r="IR8" s="46"/>
-    </row>
-    <row r="9" spans="1:252">
+      <c r="IP8" s="92"/>
+      <c r="IQ8" s="92"/>
+      <c r="IR8" s="92"/>
+      <c r="IS8" s="92"/>
+      <c r="IT8" s="92"/>
+      <c r="IU8" s="92"/>
+    </row>
+    <row r="9" spans="1:255">
       <c r="A9" s="55"/>
       <c r="B9" s="55" t="s">
         <v>505</v>
       </c>
-      <c r="C9" s="69">
-        <v>0</v>
-      </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="70" t="s">
+      <c r="C9" s="93">
+        <v>0</v>
+      </c>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="94" t="s">
         <v>512</v>
       </c>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="69">
-        <v>0</v>
-      </c>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="66" t="s">
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="93">
+        <v>0</v>
+      </c>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="68" t="s">
         <v>512</v>
       </c>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="68"/>
-      <c r="R9" s="69">
-        <v>0</v>
-      </c>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="V9" s="70" t="s">
+      <c r="P9" s="69"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="93">
+        <v>0</v>
+      </c>
+      <c r="S9" s="93"/>
+      <c r="T9" s="93"/>
+      <c r="U9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="94" t="s">
         <v>512</v>
       </c>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z9" s="69">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="69"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD9" s="66" t="s">
+      <c r="W9" s="94"/>
+      <c r="X9" s="94"/>
+      <c r="Y9" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z9" s="93">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="93"/>
+      <c r="AB9" s="93"/>
+      <c r="AC9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD9" s="68" t="s">
         <v>512</v>
       </c>
-      <c r="AE9" s="67"/>
-      <c r="AF9" s="68"/>
-      <c r="AG9" s="69">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="69"/>
-      <c r="AI9" s="69"/>
-      <c r="AJ9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK9" s="70" t="s">
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="93">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="93"/>
+      <c r="AI9" s="93"/>
+      <c r="AJ9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK9" s="94" t="s">
         <v>512</v>
       </c>
-      <c r="AL9" s="70"/>
-      <c r="AM9" s="70"/>
-      <c r="AN9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO9" s="69">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="69"/>
-      <c r="AQ9" s="69"/>
-      <c r="AR9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS9" s="66" t="s">
+      <c r="AL9" s="94"/>
+      <c r="AM9" s="94"/>
+      <c r="AN9" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO9" s="93">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="93"/>
+      <c r="AQ9" s="93"/>
+      <c r="AR9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS9" s="68" t="s">
         <v>512</v>
       </c>
-      <c r="AT9" s="67"/>
-      <c r="AU9" s="68"/>
-      <c r="AV9" s="72">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="72"/>
-      <c r="AX9" s="72"/>
-      <c r="AY9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AZ9" s="71">
-        <v>255</v>
-      </c>
-      <c r="BA9" s="71"/>
-      <c r="BB9" s="71"/>
-      <c r="BC9" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="BD9" s="72">
-        <v>0</v>
-      </c>
-      <c r="BE9" s="72"/>
-      <c r="BF9" s="72"/>
-      <c r="BG9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BH9" s="71">
-        <v>255</v>
-      </c>
-      <c r="BI9" s="71"/>
-      <c r="BJ9" s="71"/>
-      <c r="BK9" s="72">
-        <v>0</v>
-      </c>
-      <c r="BL9" s="72"/>
-      <c r="BM9" s="72"/>
-      <c r="BN9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BO9" s="71">
-        <v>255</v>
-      </c>
-      <c r="BP9" s="71"/>
-      <c r="BQ9" s="71"/>
-      <c r="BR9" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="BS9" s="72">
-        <v>0</v>
-      </c>
-      <c r="BT9" s="72"/>
-      <c r="BU9" s="72"/>
-      <c r="BV9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BW9" s="71">
-        <v>255</v>
-      </c>
-      <c r="BX9" s="71"/>
-      <c r="BY9" s="71"/>
-      <c r="BZ9" s="69">
-        <v>0</v>
-      </c>
-      <c r="CA9" s="69"/>
-      <c r="CB9" s="69"/>
-      <c r="CC9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CD9" s="70" t="s">
+      <c r="AT9" s="69"/>
+      <c r="AU9" s="70"/>
+      <c r="AV9" s="77">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="77"/>
+      <c r="AX9" s="77"/>
+      <c r="AY9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ9" s="95" t="s">
+        <v>512</v>
+      </c>
+      <c r="BA9" s="95"/>
+      <c r="BB9" s="95"/>
+      <c r="BC9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="BD9" s="77">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="77"/>
+      <c r="BF9" s="77"/>
+      <c r="BG9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH9" s="78" t="s">
+        <v>512</v>
+      </c>
+      <c r="BI9" s="78"/>
+      <c r="BJ9" s="78"/>
+      <c r="BK9" s="77">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="77"/>
+      <c r="BM9" s="77"/>
+      <c r="BN9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BO9" s="78" t="s">
+        <v>512</v>
+      </c>
+      <c r="BP9" s="78"/>
+      <c r="BQ9" s="78"/>
+      <c r="BR9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="BS9" s="77">
+        <v>0</v>
+      </c>
+      <c r="BT9" s="77"/>
+      <c r="BU9" s="77"/>
+      <c r="BV9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BW9" s="78" t="s">
+        <v>512</v>
+      </c>
+      <c r="BX9" s="78"/>
+      <c r="BY9" s="78"/>
+      <c r="BZ9" s="93">
+        <v>0</v>
+      </c>
+      <c r="CA9" s="93"/>
+      <c r="CB9" s="93"/>
+      <c r="CC9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CD9" s="96" t="s">
         <v>514</v>
       </c>
-      <c r="CE9" s="70"/>
-      <c r="CF9" s="70"/>
-      <c r="CG9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CH9" s="69">
-        <v>0</v>
-      </c>
-      <c r="CI9" s="69"/>
-      <c r="CJ9" s="69"/>
-      <c r="CK9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CL9" s="66" t="s">
+      <c r="CE9" s="96"/>
+      <c r="CF9" s="96"/>
+      <c r="CG9" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="CH9" s="93">
+        <v>0</v>
+      </c>
+      <c r="CI9" s="93"/>
+      <c r="CJ9" s="93"/>
+      <c r="CK9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CL9" s="74" t="s">
         <v>514</v>
       </c>
-      <c r="CM9" s="67"/>
-      <c r="CN9" s="68"/>
-      <c r="CO9" s="69">
-        <v>0</v>
-      </c>
-      <c r="CP9" s="69"/>
-      <c r="CQ9" s="69"/>
-      <c r="CR9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CS9" s="70" t="s">
+      <c r="CM9" s="75"/>
+      <c r="CN9" s="76"/>
+      <c r="CO9" s="93">
+        <v>0</v>
+      </c>
+      <c r="CP9" s="93"/>
+      <c r="CQ9" s="93"/>
+      <c r="CR9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CS9" s="96" t="s">
         <v>514</v>
       </c>
-      <c r="CT9" s="70"/>
-      <c r="CU9" s="70"/>
-      <c r="CV9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CW9" s="69">
-        <v>0</v>
-      </c>
-      <c r="CX9" s="69"/>
-      <c r="CY9" s="69"/>
-      <c r="CZ9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DA9" s="66" t="s">
+      <c r="CT9" s="96"/>
+      <c r="CU9" s="96"/>
+      <c r="CV9" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="CW9" s="93">
+        <v>0</v>
+      </c>
+      <c r="CX9" s="93"/>
+      <c r="CY9" s="93"/>
+      <c r="CZ9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DA9" s="74" t="s">
         <v>514</v>
       </c>
-      <c r="DB9" s="67"/>
-      <c r="DC9" s="68"/>
-      <c r="DD9" s="69">
-        <v>0</v>
-      </c>
-      <c r="DE9" s="69"/>
-      <c r="DF9" s="69"/>
-      <c r="DG9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DH9" s="70" t="s">
+      <c r="DB9" s="75"/>
+      <c r="DC9" s="76"/>
+      <c r="DD9" s="93">
+        <v>0</v>
+      </c>
+      <c r="DE9" s="93"/>
+      <c r="DF9" s="93"/>
+      <c r="DG9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DH9" s="96" t="s">
         <v>517</v>
       </c>
-      <c r="DI9" s="70"/>
-      <c r="DJ9" s="70"/>
-      <c r="DK9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DL9" s="69">
-        <v>0</v>
-      </c>
-      <c r="DM9" s="69"/>
-      <c r="DN9" s="69"/>
-      <c r="DO9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DP9" s="70" t="s">
+      <c r="DI9" s="96"/>
+      <c r="DJ9" s="96"/>
+      <c r="DK9" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="DL9" s="93">
+        <v>0</v>
+      </c>
+      <c r="DM9" s="93"/>
+      <c r="DN9" s="93"/>
+      <c r="DO9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DP9" s="96" t="s">
         <v>517</v>
       </c>
-      <c r="DQ9" s="70"/>
-      <c r="DR9" s="70"/>
-      <c r="DS9" s="1">
-        <v>0</v>
-      </c>
-      <c r="DT9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DU9" s="1" t="s">
+      <c r="DQ9" s="96"/>
+      <c r="DR9" s="96"/>
+      <c r="DS9" s="71">
+        <v>0</v>
+      </c>
+      <c r="DT9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="DU9" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="DV9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DW9" s="1">
-        <v>0</v>
-      </c>
-      <c r="DX9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DY9" s="1" t="s">
+      <c r="DV9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="DW9" s="71">
+        <v>0</v>
+      </c>
+      <c r="DX9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="DY9" s="106" t="s">
         <v>514</v>
       </c>
-      <c r="DZ9" s="1">
-        <v>0</v>
-      </c>
-      <c r="EA9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EB9" s="1" t="s">
+      <c r="DZ9" s="109"/>
+      <c r="EA9" s="109"/>
+      <c r="EB9" s="109"/>
+      <c r="EC9" s="107">
+        <v>0</v>
+      </c>
+      <c r="ED9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="EE9" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="EC9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ED9" s="1">
-        <v>0</v>
-      </c>
-      <c r="EE9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EF9" s="1" t="s">
+      <c r="EF9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="EG9" s="71">
+        <v>0</v>
+      </c>
+      <c r="EH9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="EI9" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="EG9" s="1">
-        <v>0</v>
-      </c>
-      <c r="EH9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EI9" s="1" t="s">
+      <c r="EJ9" s="97">
+        <v>0</v>
+      </c>
+      <c r="EK9" s="98"/>
+      <c r="EL9" s="99"/>
+      <c r="EM9" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="EN9" s="83" t="s">
+        <v>519</v>
+      </c>
+      <c r="EO9" s="84"/>
+      <c r="EP9" s="85"/>
+      <c r="EQ9" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="ER9" s="97">
+        <v>0</v>
+      </c>
+      <c r="ES9" s="98"/>
+      <c r="ET9" s="99"/>
+      <c r="EU9" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="EV9" s="83" t="s">
+        <v>519</v>
+      </c>
+      <c r="EW9" s="84"/>
+      <c r="EX9" s="85"/>
+      <c r="EY9" s="77">
+        <v>0</v>
+      </c>
+      <c r="EZ9" s="77"/>
+      <c r="FA9" s="77"/>
+      <c r="FB9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FC9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="EJ9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EK9" s="1">
-        <v>0</v>
-      </c>
-      <c r="EL9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EM9" s="1" t="s">
+      <c r="FD9" s="78"/>
+      <c r="FE9" s="78"/>
+      <c r="FF9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FG9" s="77">
+        <v>0</v>
+      </c>
+      <c r="FH9" s="77"/>
+      <c r="FI9" s="77"/>
+      <c r="FJ9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FK9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="EN9" s="1">
-        <v>0</v>
-      </c>
-      <c r="EQ9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ER9" s="1" t="s">
+      <c r="FL9" s="78"/>
+      <c r="FM9" s="78"/>
+      <c r="FN9" s="77">
+        <v>0</v>
+      </c>
+      <c r="FO9" s="77"/>
+      <c r="FP9" s="77"/>
+      <c r="FQ9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FR9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="EU9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EV9" s="1">
-        <v>0</v>
-      </c>
-      <c r="EY9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EZ9" s="1" t="s">
+      <c r="FS9" s="78"/>
+      <c r="FT9" s="78"/>
+      <c r="FU9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FV9" s="77">
+        <v>0</v>
+      </c>
+      <c r="FW9" s="77"/>
+      <c r="FX9" s="77"/>
+      <c r="FY9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FZ9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="FC9" s="1">
-        <v>0</v>
-      </c>
-      <c r="FF9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FG9" s="1" t="s">
+      <c r="GA9" s="78"/>
+      <c r="GB9" s="78"/>
+      <c r="GC9" s="77">
+        <v>0</v>
+      </c>
+      <c r="GD9" s="77"/>
+      <c r="GE9" s="77"/>
+      <c r="GF9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="FJ9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FK9" s="1">
-        <v>0</v>
-      </c>
-      <c r="FN9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FO9" s="1" t="s">
+      <c r="GH9" s="78"/>
+      <c r="GI9" s="78"/>
+      <c r="GJ9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK9" s="77">
+        <v>0</v>
+      </c>
+      <c r="GL9" s="77"/>
+      <c r="GM9" s="77"/>
+      <c r="GN9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GO9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="FR9" s="1">
-        <v>0</v>
-      </c>
-      <c r="FU9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FV9" s="1" t="s">
+      <c r="GP9" s="78"/>
+      <c r="GQ9" s="78"/>
+      <c r="GR9" s="71">
+        <v>0</v>
+      </c>
+      <c r="GS9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GT9" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FY9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FZ9" s="1">
-        <v>0</v>
-      </c>
-      <c r="GC9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GD9" s="1" t="s">
+      <c r="GU9" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="GV9" s="71">
+        <v>0</v>
+      </c>
+      <c r="GW9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GX9" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="GG9" s="1">
-        <v>0</v>
-      </c>
-      <c r="GJ9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GK9" s="1" t="s">
+      <c r="GY9" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="GZ9" s="88">
+        <v>0</v>
+      </c>
+      <c r="HA9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="HB9" s="89" t="s">
         <v>514</v>
       </c>
-      <c r="GN9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GO9" s="1">
-        <v>0</v>
-      </c>
-      <c r="GR9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GS9" s="1" t="s">
+      <c r="HC9" s="77">
+        <v>0</v>
+      </c>
+      <c r="HD9" s="77"/>
+      <c r="HE9" s="77"/>
+      <c r="HF9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HG9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="GV9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GW9" s="1">
-        <v>0</v>
-      </c>
-      <c r="GX9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GY9" s="1" t="s">
+      <c r="HH9" s="78"/>
+      <c r="HI9" s="78"/>
+      <c r="HJ9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="HK9" s="77">
+        <v>0</v>
+      </c>
+      <c r="HL9" s="77"/>
+      <c r="HM9" s="77"/>
+      <c r="HN9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HO9" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="GZ9" s="1">
-        <v>0</v>
-      </c>
-      <c r="HC9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HD9" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="HG9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HH9" s="1">
-        <v>0</v>
-      </c>
-      <c r="HK9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HL9" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="HO9" s="1">
-        <v>0</v>
-      </c>
-      <c r="HR9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HS9" s="1" t="s">
+      <c r="HP9" s="78"/>
+      <c r="HQ9" s="78"/>
+      <c r="HR9" s="77">
+        <v>0</v>
+      </c>
+      <c r="HS9" s="77"/>
+      <c r="HT9" s="77"/>
+      <c r="HU9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HV9" s="78" t="s">
         <v>512</v>
       </c>
-      <c r="HV9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HW9" s="1">
-        <v>0</v>
-      </c>
-      <c r="HZ9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="IA9" s="1" t="s">
+      <c r="HW9" s="78"/>
+      <c r="HX9" s="78"/>
+      <c r="HY9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="HZ9" s="77">
+        <v>0</v>
+      </c>
+      <c r="IA9" s="77"/>
+      <c r="IB9" s="77"/>
+      <c r="IC9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="ID9" s="78" t="s">
         <v>512</v>
       </c>
-      <c r="ID9" s="45">
-        <v>0</v>
-      </c>
-      <c r="IE9" s="46"/>
-      <c r="IF9" s="46"/>
-      <c r="IG9" s="45" t="s">
+      <c r="IE9" s="78"/>
+      <c r="IF9" s="78"/>
+      <c r="IG9" s="77">
+        <v>0</v>
+      </c>
+      <c r="IH9" s="77"/>
+      <c r="II9" s="77"/>
+      <c r="IJ9" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="IK9" s="78" t="s">
+        <v>512</v>
+      </c>
+      <c r="IL9" s="78"/>
+      <c r="IM9" s="78"/>
+      <c r="IN9" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="IH9" s="45" t="s">
+      <c r="IO9" s="101">
+        <v>0</v>
+      </c>
+      <c r="IP9" s="101"/>
+      <c r="IQ9" s="101"/>
+      <c r="IR9" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="IS9" s="102" t="s">
         <v>512</v>
       </c>
-      <c r="II9" s="46"/>
-      <c r="IJ9" s="46"/>
-      <c r="IK9" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="IL9" s="45">
-        <v>0</v>
-      </c>
-      <c r="IM9" s="46"/>
-      <c r="IN9" s="46"/>
-      <c r="IO9" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="IP9" s="45" t="s">
-        <v>512</v>
-      </c>
-      <c r="IQ9" s="46"/>
-      <c r="IR9" s="46"/>
-    </row>
-    <row r="10" spans="1:252">
+      <c r="IT9" s="102"/>
+      <c r="IU9" s="102"/>
+    </row>
+    <row r="10" spans="1:255">
       <c r="A10" s="55"/>
       <c r="B10" s="55" t="s">
         <v>506</v>
       </c>
-      <c r="C10" s="56">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="88">
+        <v>0</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="56">
-        <v>0</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="13" t="s">
+      <c r="F10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="88">
+        <v>0</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="56">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="13" t="s">
+      <c r="J10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="88">
+        <v>0</v>
+      </c>
+      <c r="L10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="56">
-        <v>0</v>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="13" t="s">
+      <c r="N10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="88">
+        <v>0</v>
+      </c>
+      <c r="P10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="R10" s="56">
-        <v>0</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="T10" s="13" t="s">
+      <c r="R10" s="88">
+        <v>0</v>
+      </c>
+      <c r="S10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="U10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V10" s="56">
-        <v>0</v>
-      </c>
-      <c r="W10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="X10" s="13" t="s">
+      <c r="U10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="V10" s="88">
+        <v>0</v>
+      </c>
+      <c r="W10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="X10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="Y10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z10" s="56">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB10" s="13" t="s">
+      <c r="Y10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z10" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="AC10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD10" s="56">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF10" s="13" t="s">
+      <c r="AC10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD10" s="88">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="AG10" s="56">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI10" s="13" t="s">
+      <c r="AG10" s="88">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="AJ10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK10" s="56">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM10" s="13" t="s">
+      <c r="AJ10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK10" s="88">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="AN10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO10" s="56">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ10" s="13" t="s">
+      <c r="AN10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO10" s="88">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="AR10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS10" s="56">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AU10" s="13" t="s">
+      <c r="AR10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS10" s="88">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU10" s="103" t="s">
         <v>512</v>
       </c>
-      <c r="AV10" s="72">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="72"/>
-      <c r="AX10" s="72"/>
-      <c r="AY10" s="72"/>
-      <c r="AZ10" s="72"/>
-      <c r="BA10" s="72"/>
-      <c r="BB10" s="72"/>
-      <c r="BC10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BD10" s="71">
-        <v>4</v>
-      </c>
-      <c r="BE10" s="71"/>
-      <c r="BF10" s="71"/>
-      <c r="BG10" s="71"/>
-      <c r="BH10" s="71"/>
-      <c r="BI10" s="71"/>
-      <c r="BJ10" s="71"/>
-      <c r="BK10" s="72">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="72"/>
-      <c r="BM10" s="72"/>
-      <c r="BN10" s="72"/>
-      <c r="BO10" s="72"/>
-      <c r="BP10" s="72"/>
-      <c r="BQ10" s="72"/>
-      <c r="BR10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BS10" s="71" t="s">
+      <c r="AV10" s="77">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="77"/>
+      <c r="AX10" s="77"/>
+      <c r="AY10" s="77"/>
+      <c r="AZ10" s="77"/>
+      <c r="BA10" s="77"/>
+      <c r="BB10" s="77"/>
+      <c r="BC10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BD10" s="78" t="s">
         <v>514</v>
       </c>
-      <c r="BT10" s="71"/>
-      <c r="BU10" s="71"/>
-      <c r="BV10" s="71"/>
-      <c r="BW10" s="71"/>
-      <c r="BX10" s="71"/>
-      <c r="BY10" s="71"/>
-      <c r="BZ10" s="56">
-        <v>0</v>
-      </c>
-      <c r="CA10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CB10" s="13" t="s">
+      <c r="BE10" s="78"/>
+      <c r="BF10" s="78"/>
+      <c r="BG10" s="78"/>
+      <c r="BH10" s="78"/>
+      <c r="BI10" s="78"/>
+      <c r="BJ10" s="78"/>
+      <c r="BK10" s="77">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="77"/>
+      <c r="BM10" s="77"/>
+      <c r="BN10" s="77"/>
+      <c r="BO10" s="77"/>
+      <c r="BP10" s="77"/>
+      <c r="BQ10" s="77"/>
+      <c r="BR10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="BS10" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="BT10" s="78"/>
+      <c r="BU10" s="78"/>
+      <c r="BV10" s="78"/>
+      <c r="BW10" s="78"/>
+      <c r="BX10" s="78"/>
+      <c r="BY10" s="78"/>
+      <c r="BZ10" s="88">
+        <v>0</v>
+      </c>
+      <c r="CA10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CB10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="CC10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CD10" s="56">
-        <v>0</v>
-      </c>
-      <c r="CE10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CF10" s="13" t="s">
+      <c r="CC10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="CD10" s="88">
+        <v>0</v>
+      </c>
+      <c r="CE10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CF10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="CG10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CH10" s="56">
-        <v>0</v>
-      </c>
-      <c r="CI10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CJ10" s="13" t="s">
+      <c r="CG10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="CH10" s="88">
+        <v>0</v>
+      </c>
+      <c r="CI10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CJ10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="CK10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CL10" s="56">
-        <v>0</v>
-      </c>
-      <c r="CM10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CN10" s="13" t="s">
+      <c r="CK10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="CL10" s="88">
+        <v>0</v>
+      </c>
+      <c r="CM10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CN10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="CO10" s="56">
-        <v>0</v>
-      </c>
-      <c r="CP10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CQ10" s="13" t="s">
+      <c r="CO10" s="88">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CQ10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="CR10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CS10" s="56">
-        <v>0</v>
-      </c>
-      <c r="CT10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CU10" s="13" t="s">
+      <c r="CR10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="CS10" s="88">
+        <v>0</v>
+      </c>
+      <c r="CT10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CU10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="CV10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CW10" s="56">
-        <v>0</v>
-      </c>
-      <c r="CX10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="CY10" s="13" t="s">
+      <c r="CV10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="CW10" s="88">
+        <v>0</v>
+      </c>
+      <c r="CX10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="CY10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="CZ10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DA10" s="56">
-        <v>0</v>
-      </c>
-      <c r="DB10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DC10" s="13" t="s">
+      <c r="CZ10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="DA10" s="88">
+        <v>0</v>
+      </c>
+      <c r="DB10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DC10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="DD10" s="56">
-        <v>0</v>
-      </c>
-      <c r="DE10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DF10" s="13" t="s">
+      <c r="DD10" s="88">
+        <v>0</v>
+      </c>
+      <c r="DE10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DF10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="DG10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DH10" s="56">
-        <v>0</v>
-      </c>
-      <c r="DI10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DJ10" s="13" t="s">
+      <c r="DG10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="DH10" s="88">
+        <v>0</v>
+      </c>
+      <c r="DI10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DJ10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="DK10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DL10" s="56">
-        <v>0</v>
-      </c>
-      <c r="DM10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DN10" s="13" t="s">
+      <c r="DK10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="DL10" s="88">
+        <v>0</v>
+      </c>
+      <c r="DM10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DN10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="DO10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DP10" s="56">
-        <v>0</v>
-      </c>
-      <c r="DQ10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DR10" s="13" t="s">
+      <c r="DO10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="DP10" s="88">
+        <v>0</v>
+      </c>
+      <c r="DQ10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="DR10" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="EN10" s="1">
-        <v>0</v>
-      </c>
-      <c r="EO10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EP10" s="1" t="s">
+      <c r="DS10" s="87"/>
+      <c r="DT10" s="87"/>
+      <c r="DU10" s="87"/>
+      <c r="DV10" s="87"/>
+      <c r="DW10" s="87"/>
+      <c r="DX10" s="87"/>
+      <c r="DY10" s="87"/>
+      <c r="DZ10" s="87"/>
+      <c r="EA10" s="87"/>
+      <c r="EB10" s="87"/>
+      <c r="EC10" s="87"/>
+      <c r="ED10" s="87"/>
+      <c r="EE10" s="87"/>
+      <c r="EF10" s="87"/>
+      <c r="EG10" s="87"/>
+      <c r="EH10" s="87"/>
+      <c r="EI10" s="87"/>
+      <c r="EJ10" s="104">
+        <v>0</v>
+      </c>
+      <c r="EK10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="EL10" s="105" t="s">
+        <v>519</v>
+      </c>
+      <c r="EM10" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="EN10" s="104">
+        <v>0</v>
+      </c>
+      <c r="EO10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="EP10" s="105" t="s">
+        <v>519</v>
+      </c>
+      <c r="EQ10" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="ER10" s="104">
+        <v>0</v>
+      </c>
+      <c r="ES10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="ET10" s="105" t="s">
+        <v>519</v>
+      </c>
+      <c r="EU10" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="EV10" s="104">
+        <v>0</v>
+      </c>
+      <c r="EW10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="EX10" s="105" t="s">
+        <v>519</v>
+      </c>
+      <c r="EY10" s="71">
+        <v>0</v>
+      </c>
+      <c r="EZ10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FA10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="EQ10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ER10" s="1">
-        <v>0</v>
-      </c>
-      <c r="ES10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ET10" s="1" t="s">
+      <c r="FB10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FC10" s="71">
+        <v>0</v>
+      </c>
+      <c r="FD10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FE10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="EU10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EV10" s="1">
-        <v>0</v>
-      </c>
-      <c r="EW10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EX10" s="1" t="s">
+      <c r="FF10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FG10" s="71">
+        <v>0</v>
+      </c>
+      <c r="FH10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FI10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="EY10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EZ10" s="1">
-        <v>0</v>
-      </c>
-      <c r="FA10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FB10" s="1" t="s">
+      <c r="FJ10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FK10" s="71">
+        <v>0</v>
+      </c>
+      <c r="FL10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FM10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FC10" s="1">
-        <v>0</v>
-      </c>
-      <c r="FD10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FE10" s="1" t="s">
+      <c r="FN10" s="71">
+        <v>0</v>
+      </c>
+      <c r="FO10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FF10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FG10" s="1">
-        <v>0</v>
-      </c>
-      <c r="FH10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FI10" s="1" t="s">
+      <c r="FQ10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FR10" s="71">
+        <v>0</v>
+      </c>
+      <c r="FS10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FJ10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FK10" s="1">
-        <v>0</v>
-      </c>
-      <c r="FL10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FM10" s="1" t="s">
+      <c r="FU10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FV10" s="71">
+        <v>0</v>
+      </c>
+      <c r="FW10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="FX10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FN10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FO10" s="1">
-        <v>0</v>
-      </c>
-      <c r="FP10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FQ10" s="1" t="s">
+      <c r="FY10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="FZ10" s="71">
+        <v>0</v>
+      </c>
+      <c r="GA10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GB10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FR10" s="1">
-        <v>0</v>
-      </c>
-      <c r="FS10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FT10" s="1" t="s">
+      <c r="GC10" s="71">
+        <v>0</v>
+      </c>
+      <c r="GD10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GE10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FU10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FV10" s="1">
-        <v>0</v>
-      </c>
-      <c r="FW10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FX10" s="1" t="s">
+      <c r="GF10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="GG10" s="71">
+        <v>0</v>
+      </c>
+      <c r="GH10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GI10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="FY10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FZ10" s="1">
-        <v>0</v>
-      </c>
-      <c r="GA10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GB10" s="1" t="s">
+      <c r="GJ10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="GK10" s="71">
+        <v>0</v>
+      </c>
+      <c r="GL10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GM10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="GC10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GD10" s="1">
-        <v>0</v>
-      </c>
-      <c r="GE10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GF10" s="1" t="s">
+      <c r="GN10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="GO10" s="71">
+        <v>0</v>
+      </c>
+      <c r="GP10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="GQ10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="GG10" s="1">
-        <v>0</v>
-      </c>
-      <c r="GH10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GI10" s="1" t="s">
+      <c r="GR10" s="108"/>
+      <c r="GS10" s="108"/>
+      <c r="GT10" s="108"/>
+      <c r="GU10" s="108"/>
+      <c r="GV10" s="108"/>
+      <c r="GW10" s="108"/>
+      <c r="GX10" s="108"/>
+      <c r="GY10" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="GZ10" s="88">
+        <v>0</v>
+      </c>
+      <c r="HA10" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="HB10" s="89" t="s">
         <v>514</v>
       </c>
-      <c r="GJ10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GK10" s="1">
-        <v>0</v>
-      </c>
-      <c r="GL10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GM10" s="1" t="s">
+      <c r="HC10" s="71">
+        <v>0</v>
+      </c>
+      <c r="HD10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HE10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="GN10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GO10" s="1">
-        <v>0</v>
-      </c>
-      <c r="GP10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GQ10" s="1" t="s">
+      <c r="HF10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="HG10" s="71">
+        <v>0</v>
+      </c>
+      <c r="HH10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HI10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="GR10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GS10" s="1">
-        <v>0</v>
-      </c>
-      <c r="GT10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GU10" s="1" t="s">
+      <c r="HJ10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="HK10" s="71">
+        <v>0</v>
+      </c>
+      <c r="HL10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HM10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="GV10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GW10" s="1">
-        <v>0</v>
-      </c>
-      <c r="GX10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GY10" s="1" t="s">
+      <c r="HN10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="HO10" s="71">
+        <v>0</v>
+      </c>
+      <c r="HP10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HQ10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="GZ10" s="1">
-        <v>0</v>
-      </c>
-      <c r="HA10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HB10" s="1" t="s">
+      <c r="HR10" s="71">
+        <v>0</v>
+      </c>
+      <c r="HS10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HT10" s="73" t="s">
+        <v>517</v>
+      </c>
+      <c r="HU10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="HV10" s="71">
+        <v>0</v>
+      </c>
+      <c r="HW10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="HX10" s="73" t="s">
+        <v>517</v>
+      </c>
+      <c r="HY10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="HZ10" s="71">
+        <v>0</v>
+      </c>
+      <c r="IA10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="IB10" s="73" t="s">
+        <v>517</v>
+      </c>
+      <c r="IC10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="ID10" s="71">
+        <v>0</v>
+      </c>
+      <c r="IE10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="IF10" s="73" t="s">
+        <v>517</v>
+      </c>
+      <c r="IG10" s="71">
+        <v>0</v>
+      </c>
+      <c r="IH10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="II10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="HC10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HD10" s="1">
-        <v>0</v>
-      </c>
-      <c r="HE10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HF10" s="1" t="s">
+      <c r="IJ10" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="IK10" s="71">
+        <v>0</v>
+      </c>
+      <c r="IL10" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="IM10" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="HG10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HH10" s="1">
-        <v>0</v>
-      </c>
-      <c r="HI10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HJ10" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="HK10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HL10" s="1">
-        <v>0</v>
-      </c>
-      <c r="HM10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HN10" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="HO10" s="1">
-        <v>0</v>
-      </c>
-      <c r="HP10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HQ10" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="HR10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HS10" s="1">
-        <v>0</v>
-      </c>
-      <c r="HT10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HU10" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="HV10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HW10" s="1">
-        <v>0</v>
-      </c>
-      <c r="HX10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HY10" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="HZ10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="IA10" s="1">
-        <v>0</v>
-      </c>
-      <c r="IB10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="IC10" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="ID10" s="45">
-        <v>0</v>
-      </c>
-      <c r="IE10" s="45" t="s">
+      <c r="IN10" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="IF10" s="45" t="s">
+      <c r="IO10" s="104">
+        <v>0</v>
+      </c>
+      <c r="IP10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="IQ10" s="105" t="s">
         <v>519</v>
       </c>
-      <c r="IG10" s="45" t="s">
+      <c r="IR10" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="IH10" s="45">
-        <v>0</v>
-      </c>
-      <c r="II10" s="45" t="s">
+      <c r="IS10" s="104">
+        <v>0</v>
+      </c>
+      <c r="IT10" s="82" t="s">
         <v>87</v>
       </c>
-      <c r="IJ10" s="45" t="s">
+      <c r="IU10" s="105" t="s">
         <v>519</v>
       </c>
-      <c r="IK10" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="IL10" s="45">
-        <v>0</v>
-      </c>
-      <c r="IM10" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="IN10" s="45" t="s">
-        <v>519</v>
-      </c>
-      <c r="IO10" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="IP10" s="45">
-        <v>0</v>
-      </c>
-      <c r="IQ10" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="IR10" s="45" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="11" spans="1:252">
+    </row>
+    <row r="11" spans="1:255">
       <c r="A11" s="2"/>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="55" t="s">
         <v>520</v>
       </c>
-      <c r="EN11" s="1">
-        <v>0</v>
-      </c>
-      <c r="GV11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GW11" s="1">
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="87"/>
+      <c r="T11" s="87"/>
+      <c r="U11" s="87"/>
+      <c r="V11" s="87"/>
+      <c r="W11" s="87"/>
+      <c r="X11" s="87"/>
+      <c r="Y11" s="87"/>
+      <c r="Z11" s="87"/>
+      <c r="AA11" s="87"/>
+      <c r="AB11" s="87"/>
+      <c r="AC11" s="87"/>
+      <c r="AD11" s="87"/>
+      <c r="AE11" s="87"/>
+      <c r="AF11" s="87"/>
+      <c r="AG11" s="87"/>
+      <c r="AH11" s="87"/>
+      <c r="AI11" s="87"/>
+      <c r="AJ11" s="87"/>
+      <c r="AK11" s="87"/>
+      <c r="AL11" s="87"/>
+      <c r="AM11" s="87"/>
+      <c r="AN11" s="87"/>
+      <c r="AO11" s="87"/>
+      <c r="AP11" s="87"/>
+      <c r="AQ11" s="87"/>
+      <c r="AR11" s="87"/>
+      <c r="AS11" s="87"/>
+      <c r="AT11" s="87"/>
+      <c r="AU11" s="87"/>
+      <c r="AV11" s="87"/>
+      <c r="AW11" s="87"/>
+      <c r="AX11" s="87"/>
+      <c r="AY11" s="87"/>
+      <c r="AZ11" s="87"/>
+      <c r="BA11" s="87"/>
+      <c r="BB11" s="87"/>
+      <c r="BC11" s="87"/>
+      <c r="BD11" s="87"/>
+      <c r="BE11" s="87"/>
+      <c r="BF11" s="87"/>
+      <c r="BG11" s="87"/>
+      <c r="BH11" s="87"/>
+      <c r="BI11" s="87"/>
+      <c r="BJ11" s="87"/>
+      <c r="BK11" s="87"/>
+      <c r="BL11" s="87"/>
+      <c r="BM11" s="87"/>
+      <c r="BN11" s="87"/>
+      <c r="BO11" s="87"/>
+      <c r="BP11" s="87"/>
+      <c r="BQ11" s="87"/>
+      <c r="BR11" s="87"/>
+      <c r="BS11" s="87"/>
+      <c r="BT11" s="87"/>
+      <c r="BU11" s="87"/>
+      <c r="BV11" s="87"/>
+      <c r="BW11" s="87"/>
+      <c r="BX11" s="87"/>
+      <c r="BY11" s="87"/>
+      <c r="BZ11" s="87"/>
+      <c r="CA11" s="87"/>
+      <c r="CB11" s="87"/>
+      <c r="CC11" s="87"/>
+      <c r="CD11" s="87"/>
+      <c r="CE11" s="87"/>
+      <c r="CF11" s="87"/>
+      <c r="CG11" s="87"/>
+      <c r="CH11" s="87"/>
+      <c r="CI11" s="87"/>
+      <c r="CJ11" s="87"/>
+      <c r="CK11" s="87"/>
+      <c r="CL11" s="87"/>
+      <c r="CM11" s="87"/>
+      <c r="CN11" s="87"/>
+      <c r="CO11" s="87"/>
+      <c r="CP11" s="87"/>
+      <c r="CQ11" s="87"/>
+      <c r="CR11" s="87"/>
+      <c r="CS11" s="87"/>
+      <c r="CT11" s="87"/>
+      <c r="CU11" s="87"/>
+      <c r="CV11" s="87"/>
+      <c r="CW11" s="87"/>
+      <c r="CX11" s="87"/>
+      <c r="CY11" s="87"/>
+      <c r="CZ11" s="87"/>
+      <c r="DA11" s="87"/>
+      <c r="DB11" s="87"/>
+      <c r="DC11" s="87"/>
+      <c r="DD11" s="87"/>
+      <c r="DE11" s="87"/>
+      <c r="DF11" s="87"/>
+      <c r="DG11" s="87"/>
+      <c r="DH11" s="87"/>
+      <c r="DI11" s="87"/>
+      <c r="DJ11" s="87"/>
+      <c r="DK11" s="87"/>
+      <c r="DL11" s="87"/>
+      <c r="DM11" s="87"/>
+      <c r="DN11" s="87"/>
+      <c r="DO11" s="87"/>
+      <c r="DP11" s="87"/>
+      <c r="DQ11" s="87"/>
+      <c r="DR11" s="87"/>
+      <c r="DS11" s="87"/>
+      <c r="DT11" s="87"/>
+      <c r="DU11" s="87"/>
+      <c r="DV11" s="87"/>
+      <c r="DW11" s="87"/>
+      <c r="DX11" s="87"/>
+      <c r="DY11" s="87"/>
+      <c r="DZ11" s="87"/>
+      <c r="EA11" s="87"/>
+      <c r="EB11" s="87"/>
+      <c r="EC11" s="87"/>
+      <c r="ED11" s="87"/>
+      <c r="EE11" s="87"/>
+      <c r="EF11" s="87"/>
+      <c r="EG11" s="87"/>
+      <c r="EH11" s="87"/>
+      <c r="EI11" s="87"/>
+      <c r="EJ11" s="77">
+        <v>0</v>
+      </c>
+      <c r="EK11" s="77"/>
+      <c r="EL11" s="77"/>
+      <c r="EM11" s="77"/>
+      <c r="EN11" s="77"/>
+      <c r="EO11" s="77"/>
+      <c r="EP11" s="77"/>
+      <c r="EQ11" s="77"/>
+      <c r="ER11" s="77"/>
+      <c r="ES11" s="77"/>
+      <c r="ET11" s="77"/>
+      <c r="EU11" s="77"/>
+      <c r="EV11" s="77"/>
+      <c r="EW11" s="77"/>
+      <c r="EX11" s="77"/>
+      <c r="EY11" s="77"/>
+      <c r="EZ11" s="77"/>
+      <c r="FA11" s="77"/>
+      <c r="FB11" s="77"/>
+      <c r="FC11" s="77"/>
+      <c r="FD11" s="77"/>
+      <c r="FE11" s="77"/>
+      <c r="FF11" s="77"/>
+      <c r="FG11" s="77"/>
+      <c r="FH11" s="77"/>
+      <c r="FI11" s="77"/>
+      <c r="FJ11" s="77"/>
+      <c r="FK11" s="77"/>
+      <c r="FL11" s="77"/>
+      <c r="FM11" s="77"/>
+      <c r="FN11" s="77"/>
+      <c r="FO11" s="77"/>
+      <c r="FP11" s="77"/>
+      <c r="FQ11" s="77"/>
+      <c r="FR11" s="77"/>
+      <c r="FS11" s="77"/>
+      <c r="FT11" s="77"/>
+      <c r="FU11" s="77"/>
+      <c r="FV11" s="77"/>
+      <c r="FW11" s="77"/>
+      <c r="FX11" s="77"/>
+      <c r="FY11" s="77"/>
+      <c r="FZ11" s="77"/>
+      <c r="GA11" s="77"/>
+      <c r="GB11" s="77"/>
+      <c r="GC11" s="77"/>
+      <c r="GD11" s="77"/>
+      <c r="GE11" s="77"/>
+      <c r="GF11" s="77"/>
+      <c r="GG11" s="77"/>
+      <c r="GH11" s="77"/>
+      <c r="GI11" s="77"/>
+      <c r="GJ11" s="77"/>
+      <c r="GK11" s="77"/>
+      <c r="GL11" s="77"/>
+      <c r="GM11" s="77"/>
+      <c r="GN11" s="77"/>
+      <c r="GO11" s="77"/>
+      <c r="GP11" s="77"/>
+      <c r="GQ11" s="77"/>
+      <c r="GR11" s="108"/>
+      <c r="GS11" s="108"/>
+      <c r="GT11" s="108"/>
+      <c r="GU11" s="108"/>
+      <c r="GV11" s="108"/>
+      <c r="GW11" s="108"/>
+      <c r="GX11" s="108"/>
+      <c r="GY11" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="GZ11" s="78">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:252">
+      <c r="HA11" s="78"/>
+      <c r="HB11" s="78"/>
+      <c r="HC11" s="87"/>
+      <c r="HD11" s="87"/>
+      <c r="HE11" s="87"/>
+      <c r="HF11" s="87"/>
+      <c r="HG11" s="87"/>
+      <c r="HH11" s="87"/>
+      <c r="HI11" s="87"/>
+      <c r="HJ11" s="87"/>
+      <c r="HK11" s="87"/>
+      <c r="HL11" s="87"/>
+      <c r="HM11" s="87"/>
+      <c r="HN11" s="87"/>
+      <c r="HO11" s="87"/>
+      <c r="HP11" s="87"/>
+      <c r="HQ11" s="87"/>
+      <c r="HR11" s="87"/>
+      <c r="HS11" s="87"/>
+      <c r="HT11" s="87"/>
+      <c r="HU11" s="87"/>
+      <c r="HV11" s="87"/>
+      <c r="HW11" s="87"/>
+      <c r="HX11" s="87"/>
+      <c r="HY11" s="87"/>
+      <c r="HZ11" s="87"/>
+      <c r="IA11" s="87"/>
+      <c r="IB11" s="87"/>
+      <c r="IC11" s="87"/>
+      <c r="ID11" s="87"/>
+      <c r="IE11" s="87"/>
+      <c r="IF11" s="87"/>
+      <c r="IG11" s="87"/>
+      <c r="IH11" s="87"/>
+      <c r="II11" s="87"/>
+      <c r="IJ11" s="87"/>
+      <c r="IK11" s="87"/>
+      <c r="IL11" s="87"/>
+      <c r="IM11" s="87"/>
+      <c r="IN11" s="87"/>
+      <c r="IO11" s="87"/>
+      <c r="IP11" s="87"/>
+      <c r="IQ11" s="87"/>
+      <c r="IR11" s="87"/>
+      <c r="IS11" s="87"/>
+      <c r="IT11" s="87"/>
+      <c r="IU11" s="87"/>
+    </row>
+    <row r="14" spans="1:255">
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:252">
+      <c r="EA14" s="110"/>
+    </row>
+    <row r="15" spans="1:255">
       <c r="B15" s="2"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
       <c r="H15"/>
     </row>
     <row r="32" spans="1:1">
@@ -9965,7 +10963,108 @@
       <c r="AN35" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="117">
+    <mergeCell ref="GR5:GX5"/>
+    <mergeCell ref="GY5:HB5"/>
+    <mergeCell ref="HC5:HQ5"/>
+    <mergeCell ref="HR5:IF5"/>
+    <mergeCell ref="IG5:IU5"/>
+    <mergeCell ref="DS5:EI5"/>
+    <mergeCell ref="EJ5:EX5"/>
+    <mergeCell ref="EY5:FM5"/>
+    <mergeCell ref="FN5:GB5"/>
+    <mergeCell ref="GC5:GQ5"/>
+    <mergeCell ref="HZ8:IF8"/>
+    <mergeCell ref="HR8:HX8"/>
+    <mergeCell ref="HK8:HQ8"/>
+    <mergeCell ref="GZ11:HB11"/>
+    <mergeCell ref="EJ11:GQ11"/>
+    <mergeCell ref="HC8:HI8"/>
+    <mergeCell ref="GK8:GQ8"/>
+    <mergeCell ref="GC8:GI8"/>
+    <mergeCell ref="FV8:GB8"/>
+    <mergeCell ref="FN8:FT8"/>
+    <mergeCell ref="EY8:FE8"/>
+    <mergeCell ref="FG8:FM8"/>
+    <mergeCell ref="EJ8:EP8"/>
+    <mergeCell ref="ER8:EX8"/>
+    <mergeCell ref="GR8:GT8"/>
+    <mergeCell ref="GV8:GX8"/>
+    <mergeCell ref="IG9:II9"/>
+    <mergeCell ref="IK9:IM9"/>
+    <mergeCell ref="IO9:IQ9"/>
+    <mergeCell ref="IS9:IU9"/>
+    <mergeCell ref="IO8:IU8"/>
+    <mergeCell ref="IG8:IM8"/>
+    <mergeCell ref="HO9:HQ9"/>
+    <mergeCell ref="HR9:HT9"/>
+    <mergeCell ref="HV9:HX9"/>
+    <mergeCell ref="HZ9:IB9"/>
+    <mergeCell ref="ID9:IF9"/>
+    <mergeCell ref="GK9:GM9"/>
+    <mergeCell ref="GO9:GQ9"/>
+    <mergeCell ref="HC9:HE9"/>
+    <mergeCell ref="HG9:HI9"/>
+    <mergeCell ref="HK9:HM9"/>
+    <mergeCell ref="FR9:FT9"/>
+    <mergeCell ref="FV9:FX9"/>
+    <mergeCell ref="FZ9:GB9"/>
+    <mergeCell ref="GC9:GE9"/>
+    <mergeCell ref="GG9:GI9"/>
+    <mergeCell ref="EY9:FA9"/>
+    <mergeCell ref="FC9:FE9"/>
+    <mergeCell ref="FG9:FI9"/>
+    <mergeCell ref="FK9:FM9"/>
+    <mergeCell ref="FN9:FP9"/>
+    <mergeCell ref="EG8:EI8"/>
+    <mergeCell ref="EJ9:EL9"/>
+    <mergeCell ref="EN9:EP9"/>
+    <mergeCell ref="ER9:ET9"/>
+    <mergeCell ref="EV9:EX9"/>
+    <mergeCell ref="DS8:DU8"/>
+    <mergeCell ref="DW8:DY8"/>
+    <mergeCell ref="EC8:EE8"/>
+    <mergeCell ref="DD5:DR5"/>
+    <mergeCell ref="DD8:DJ8"/>
+    <mergeCell ref="DL8:DR8"/>
+    <mergeCell ref="DD9:DF9"/>
+    <mergeCell ref="DH9:DJ9"/>
+    <mergeCell ref="DL9:DN9"/>
+    <mergeCell ref="DP9:DR9"/>
+    <mergeCell ref="CO5:DC5"/>
+    <mergeCell ref="CO8:CU8"/>
+    <mergeCell ref="CW8:DC8"/>
+    <mergeCell ref="CO9:CQ9"/>
+    <mergeCell ref="CS9:CU9"/>
+    <mergeCell ref="CW9:CY9"/>
+    <mergeCell ref="DA9:DC9"/>
+    <mergeCell ref="BW9:BY9"/>
+    <mergeCell ref="BK10:BQ10"/>
+    <mergeCell ref="BS10:BY10"/>
+    <mergeCell ref="BZ5:CN5"/>
+    <mergeCell ref="BZ8:CF8"/>
+    <mergeCell ref="CH8:CN8"/>
+    <mergeCell ref="BZ9:CB9"/>
+    <mergeCell ref="CD9:CF9"/>
+    <mergeCell ref="CH9:CJ9"/>
+    <mergeCell ref="CL9:CN9"/>
+    <mergeCell ref="BK5:BY5"/>
+    <mergeCell ref="AV10:BB10"/>
+    <mergeCell ref="BD10:BJ10"/>
+    <mergeCell ref="BK9:BM9"/>
+    <mergeCell ref="BO9:BQ9"/>
+    <mergeCell ref="BS9:BU9"/>
+    <mergeCell ref="AV5:BJ5"/>
+    <mergeCell ref="AV9:AX9"/>
+    <mergeCell ref="AZ9:BB9"/>
+    <mergeCell ref="BD9:BF9"/>
+    <mergeCell ref="BH9:BJ9"/>
+    <mergeCell ref="AG8:AM8"/>
+    <mergeCell ref="AO8:AU8"/>
+    <mergeCell ref="AG9:AI9"/>
+    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="AO9:AQ9"/>
+    <mergeCell ref="AS9:AU9"/>
     <mergeCell ref="AG5:AU5"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="O9:Q9"/>
@@ -9982,50 +11081,9 @@
     <mergeCell ref="Z9:AB9"/>
     <mergeCell ref="AD9:AF9"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="AG8:AM8"/>
-    <mergeCell ref="AO8:AU8"/>
-    <mergeCell ref="AG9:AI9"/>
-    <mergeCell ref="AK9:AM9"/>
-    <mergeCell ref="AO9:AQ9"/>
-    <mergeCell ref="AS9:AU9"/>
-    <mergeCell ref="AV5:BJ5"/>
-    <mergeCell ref="AV9:AX9"/>
-    <mergeCell ref="AZ9:BB9"/>
-    <mergeCell ref="BD9:BF9"/>
-    <mergeCell ref="BH9:BJ9"/>
-    <mergeCell ref="AV10:BB10"/>
-    <mergeCell ref="BD10:BJ10"/>
-    <mergeCell ref="BK9:BM9"/>
-    <mergeCell ref="BO9:BQ9"/>
-    <mergeCell ref="BS9:BU9"/>
-    <mergeCell ref="BW9:BY9"/>
-    <mergeCell ref="BK10:BQ10"/>
-    <mergeCell ref="BS10:BY10"/>
-    <mergeCell ref="BZ5:CN5"/>
-    <mergeCell ref="BZ8:CF8"/>
-    <mergeCell ref="CH8:CN8"/>
-    <mergeCell ref="BZ9:CB9"/>
-    <mergeCell ref="CD9:CF9"/>
-    <mergeCell ref="CH9:CJ9"/>
-    <mergeCell ref="CL9:CN9"/>
-    <mergeCell ref="BK5:BY5"/>
-    <mergeCell ref="CO5:DC5"/>
-    <mergeCell ref="CO8:CU8"/>
-    <mergeCell ref="CW8:DC8"/>
-    <mergeCell ref="CO9:CQ9"/>
-    <mergeCell ref="CS9:CU9"/>
-    <mergeCell ref="CW9:CY9"/>
-    <mergeCell ref="DA9:DC9"/>
-    <mergeCell ref="DD5:DR5"/>
-    <mergeCell ref="DD8:DJ8"/>
-    <mergeCell ref="DL8:DR8"/>
-    <mergeCell ref="DD9:DF9"/>
-    <mergeCell ref="DH9:DJ9"/>
-    <mergeCell ref="DL9:DN9"/>
-    <mergeCell ref="DP9:DR9"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="AV8:BY8 C8:C9 J8:K9 R8:R9 Y8:Z9 AG8:AG9 AN8:AO9 BZ8:BZ9 CG8:CH9 CO8:CO9 CV8:CW9 DD8:DD9 DK8:DL9 F9:G9 N9:O9 U9:V9 AC9:AD9 AJ9:AK9 AR9:AS9 AV9 AY9:AZ9 BG9:BH9 BN9:BO9 BV9:BW9 CC9:CD9 CK9:CL9 CR9:CS9 CZ9:DA9 DG9:DH9 DO9:DP9 BC9:BD10 BK9:BK10 BR9:BS10 C10:AV10 C11:XFD1048576 BZ10:EU10 DS8:EU9 EV8:IC10 IS8:XFD10">
+  <conditionalFormatting sqref="AV8:BY8 C8:C9 J8:K9 BZ8:BZ9 CG8:CH9 CO8:CO9 CV8:CW9 DD8:DD9 DK8:DL9 IV8:XFD10 F9:G9 N9:O9 AY9:AZ9 BG9:BH9 BN9:BO9 BV9:BW9 CC9:CD9 CK9:CL9 CR9:CS9 CZ9:DA9 DG9:DH9 DO9:DP9 BC9:BD10 BK9:BK10 BR9:BS10 DS8 DV8:DW8 DZ8 EC8 EF8:EG8 FU9:FU10 FQ9:FR9 FV9 FY9:FZ9 GY9:HB10 HJ9:HJ10 HC9 HF9:HG9 HC10:HI10 HY9:HY10 HK9 HN9:HO9 HU9:HV9 HK10:HX10 HZ9 IC9:ID9 IG9 IJ9:IK9 HZ10:IM10 HY8:HZ8 HR8:HR9 HC11:XFD11 GY11:GZ11 HJ8:HK8 GY8:HC8 FU8:FV8 GJ9:GJ10 GC8:GC9 GF9:GG9 FV10:GI10 GK9 GN9:GO9 GK10:GX10 GJ8:GK8 FN8:FN9 FF9:FF10 EY8:EY9 FB9:FC9 EY10:FE10 FG9 FJ9:FK9 FF8:FG8 FG10:FT10 R8:R9 Y8:Z9 U9:V9 AC9:AD9 AV9:AV10 AG8:AG9 AN8:AO9 AJ9:AK9 AR9:AS9 C10:AU10 C12:XFD1048576 DS9:DY9 BZ10:EI10 C11:EJ11 EC9:EI9">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C8&lt;&gt;""</formula>
     </cfRule>

</xml_diff>